<commit_message>
📧 Added email with Excel attachment functionality to main.py
</commit_message>
<xml_diff>
--- a/DFS_LIST.XLSX
+++ b/DFS_LIST.XLSX
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="379">
   <si>
     <t>Product ID</t>
   </si>
@@ -173,18 +173,6 @@
     <t>LAT 5400 NB STD 14-in (1920 x 1080) TCH CAM 1x i7Q (i7-8665U) 1.90GHz 16GB 512GB NoOPT 32MB BkLIT W10P64</t>
   </si>
   <si>
-    <t>dell-optiplex-5070-sff-000255</t>
-  </si>
-  <si>
-    <t>Dell OptiPlex 5070 SFF</t>
-  </si>
-  <si>
-    <t>1x Intel Core i5-9600 (6-Core, 3.10 GHz)</t>
-  </si>
-  <si>
-    <t>OPT 5070 SFF STD 1x i56C (i5-9600) 3.10GHz 16GB 512GB NoOPT 32MB  W10P64</t>
-  </si>
-  <si>
     <t>lenovo-thinkbook-14s-yoga-touch-no-os-000005</t>
   </si>
   <si>
@@ -269,7 +257,295 @@
     <t>OPT 3060 SFF STD 1x i56C (i5-8500) 3.00GHz 16GB 512GB NoOPT 32MB  W10P64</t>
   </si>
   <si>
-    <t>dell-optiplex-7070-sff-000230</t>
+    <t>dell-latitude-7420-touch-000059</t>
+  </si>
+  <si>
+    <t>Dell Latitude 7420 Touch</t>
+  </si>
+  <si>
+    <t>1x Intel Core i5-1145G7 (4-Core, 2.60 GHz)</t>
+  </si>
+  <si>
+    <t>64-bit Windows 10 Professional</t>
+  </si>
+  <si>
+    <t>lenovo-thinkpad-e14-gen-2-no-os-000004</t>
+  </si>
+  <si>
+    <t>Lenovo ThinkPad E14 Gen 2 - No OS</t>
+  </si>
+  <si>
+    <t>1x Intel Core i7-1165G7 (4-Core, 2.80 GHz)</t>
+  </si>
+  <si>
+    <t>TKP E14 Gen 2 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i7Q (i7-1165G7) 2.80GHz 16GB 512GB NoOPT 32MB BkLIT NoOS</t>
+  </si>
+  <si>
+    <t>dell-latitude-5420-touch-000058</t>
+  </si>
+  <si>
+    <t>Dell Latitude 5420 Touch</t>
+  </si>
+  <si>
+    <t>LAT 5420 NB STD 14-in (1920 x 1080) TCH CAM 1x i7Q (i7-1185G7) 3.00GHz 16GB 512GB NoOPT 32MB BkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-optiplex-3070-mff-000164</t>
+  </si>
+  <si>
+    <t>dell-latitude-5520-touch-000026</t>
+  </si>
+  <si>
+    <t>Dell Latitude 5520 Touch</t>
+  </si>
+  <si>
+    <t>LAT 5520 NB STD 15.6-in (1920 x 1080) TCH CAM 1x i7Q (i7-1185G7) 3.00GHz 16GB 512GB NoOPT 32MB BkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-latitude-3410-000024</t>
+  </si>
+  <si>
+    <t>Dell Latitude 3410</t>
+  </si>
+  <si>
+    <t>1x Intel Core i5-10210U (4-Core, 1.60 GHz)</t>
+  </si>
+  <si>
+    <t>LAT 3410 NB STD 14-in (1366 x 768) NoTCH CAM 1x i5Q (i5-10210U) 1.60GHz 8GB 256GB NoOPT 32MB NoBkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-precision-3561-000089</t>
+  </si>
+  <si>
+    <t>Dell Precision 3561</t>
+  </si>
+  <si>
+    <t>1x Intel Core i7-11850H (8-Core, 2.50 GHz)</t>
+  </si>
+  <si>
+    <t>PRE 3561 NB STD 15.6-in (1920 x 1080) NoTCH CAM 1x i78C (i7-11850H) 2.50GHz 16GB 512GB NoOPT 4GB BkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-latitude-7420-000282</t>
+  </si>
+  <si>
+    <t>Dell Latitude 7420</t>
+  </si>
+  <si>
+    <t>LAT 7420 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i7Q (i7-1185G7) 3.00GHz 32GB 512GB NoOPT 32MB BkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-optiplex-3090-mff-000030</t>
+  </si>
+  <si>
+    <t>Dell OptiPlex 3090 MFF</t>
+  </si>
+  <si>
+    <t>1x Intel Core i3-10105T (4-Core, 3.00 GHz)</t>
+  </si>
+  <si>
+    <t>OPT 3090 MFF STD 1x i3 (i3-10105T) 3.00GHz 8GB 256GB NoOPT 32MB  W11P64</t>
+  </si>
+  <si>
+    <t>lenovo-thinkpad-t14-no-os-000013</t>
+  </si>
+  <si>
+    <t>TKP T14 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-10210U) 1.60GHz 8GB 256GB NoOPT 32MB BkLIT NoOS</t>
+  </si>
+  <si>
+    <t>lenovo-thinkpad-t14-no-os-000015</t>
+  </si>
+  <si>
+    <t>lenovo-thinkbook-14s-yoga-touch-no-os-000008</t>
+  </si>
+  <si>
+    <t>microsoft-surface-laptop-4-touch-no-os-000006</t>
+  </si>
+  <si>
+    <t>dell-optiplex-3090-mff-000034</t>
+  </si>
+  <si>
+    <t>1x Intel Core i3-10100T (4-Core, 3.00 GHz)</t>
+  </si>
+  <si>
+    <t>OPT 3090 MFF STD 1x i3Q (i3-10100T) 3.00GHz 8GB 128GB NoOPT 32MB  W11P64</t>
+  </si>
+  <si>
+    <t>lenovo-thinkcentre-m720q-mff-000003</t>
+  </si>
+  <si>
+    <t>1x Intel Core i3-8100T (4-Core, 3.10 GHz)</t>
+  </si>
+  <si>
+    <t>TKC M720Q MFF STD 1x i3Q (i3-8100T) 3.10GHz 8GB 500GB NoOPT 32MB  W10P64</t>
+  </si>
+  <si>
+    <t>dell-optiplex-3070-mff-000112</t>
+  </si>
+  <si>
+    <t>OPT 3070 MFF STD 1x i3Q (i3-9100T) 3.10GHz 8GB 256GB NoOPT 32MB  W10P64</t>
+  </si>
+  <si>
+    <t>dell-optiplex-3060-sff-000191</t>
+  </si>
+  <si>
+    <t>dell-optiplex-3070-mff-000123</t>
+  </si>
+  <si>
+    <t>dell-latitude-5400-000493</t>
+  </si>
+  <si>
+    <t>Dell Latitude 5400</t>
+  </si>
+  <si>
+    <t>1x Intel Core i5-8365U (4-Core, 1.60 GHz)</t>
+  </si>
+  <si>
+    <t>LAT 5400 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-8365U) 1.60GHz 8GB 256GB NoOPT 32MB BkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-latitude-7400-2-in-1-touch-000081</t>
+  </si>
+  <si>
+    <t>Dell Latitude 7400 2-in-1 Touch</t>
+  </si>
+  <si>
+    <t>1x Intel Core i5-8265U (4-Core, 1.60 GHz)</t>
+  </si>
+  <si>
+    <t>LAT 7400 2-in-1 2N1 STD 1x i5Q (i5-8265U) 1.60GHz 8GB 256GB NoOPT 32MB BkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-latitude-5400-000498</t>
+  </si>
+  <si>
+    <t>dell-latitude-5490-000607</t>
+  </si>
+  <si>
+    <t>Dell Latitude 5490</t>
+  </si>
+  <si>
+    <t>1x Intel Core i5-7300U (2-Core, 2.60 GHz)</t>
+  </si>
+  <si>
+    <t>LAT 5490 NB STD 14-in (1366 x 768) NoTCH CAM 1x i5 (i5-7300U) 2.60GHz 8GB 500GB NoOPT 32MB NoBkLIT W10P64</t>
+  </si>
+  <si>
+    <t>hp-zbook-15-g7-firefly-no-os-000001</t>
+  </si>
+  <si>
+    <t>HP Zbook 15 G7 FIREFLY - No OS</t>
+  </si>
+  <si>
+    <t>ZBK 15 G7 FIREFLY NB STD 15.6-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-10210U) 1.60GHz 16GB 512GB NoOPT 32MB BkLIT NoOS</t>
+  </si>
+  <si>
+    <t>dell-latitude-5400-000510</t>
+  </si>
+  <si>
+    <t>LAT 5400 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-8265U) 1.60GHz 8GB 256GB NoOPT 32MB BkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-latitude-5310-touch-000045</t>
+  </si>
+  <si>
+    <t>32 GB (2x 16GB)</t>
+  </si>
+  <si>
+    <t>LAT 5310 NB STD 13.3-in (1920 x 1080) TCH CAM 1x i5Q (i5-10310U) 1.70GHz 32GB 256GB NoOPT 32MB BkLIT W10P64</t>
+  </si>
+  <si>
+    <t>lenovo-thinkpad-t14-no-os-000010</t>
+  </si>
+  <si>
+    <t>1x Intel Core i7-10610U (4-Core, 1.80 GHz)</t>
+  </si>
+  <si>
+    <t>TKP T14 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i7Q (i7-10610U) 1.80GHz 16GB 512GB NoOPT 32MB BkLIT NoOS</t>
+  </si>
+  <si>
+    <t>dell-latitude-5490-touch-000055</t>
+  </si>
+  <si>
+    <t>Dell Latitude 5490 Touch</t>
+  </si>
+  <si>
+    <t>1x Intel Core i5-8350U (4-Core, 1.70 GHz)</t>
+  </si>
+  <si>
+    <t>LAT 5490 NB STD 14-in (1920 x 1080) TCH CAM 1x i5Q (i5-8350U) 1.70GHz 8GB 500GB NoOPT 32MB NoBkLIT W10P64</t>
+  </si>
+  <si>
+    <t>lenovo-thinkpad-t14-no-os-000012</t>
+  </si>
+  <si>
+    <t>dell-latitude-5420-000420</t>
+  </si>
+  <si>
+    <t>Dell Latitude 5420</t>
+  </si>
+  <si>
+    <t>LAT 5420 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-1135G7) 2.40GHz 8GB 256GB NoOPT 32MB BkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-latitude-5420-000431</t>
+  </si>
+  <si>
+    <t>LAT 5420 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i7Q (i7-1185G7) 3.00GHz 32GB 512GB NoOPT 32MB BkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-latitude-5410-000457</t>
+  </si>
+  <si>
+    <t>LAT 5410 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-10310U) 1.70GHz 16GB 256GB NoOPT 32MB BkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-latitude-5420-000440</t>
+  </si>
+  <si>
+    <t>LAT 5420 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-1145G7) 2.60GHz 16GB 512GB NoOPT 32MB NoBkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-optiplex-3080-sff-000144</t>
+  </si>
+  <si>
+    <t>Dell OptiPlex 3080 SFF</t>
+  </si>
+  <si>
+    <t>1x Intel Celeron G5900 (2-Core, 3.40 GHz)</t>
+  </si>
+  <si>
+    <t>24 GB (1x 8GB, 1x 16GB)</t>
+  </si>
+  <si>
+    <t>OPT 3080 SFF STD 1x CDC (G5900) 3.40GHz 24GB 256GB NoOPT 32MB  W10P64</t>
+  </si>
+  <si>
+    <t>dell-latitude-3420-000030</t>
+  </si>
+  <si>
+    <t>LAT 3420 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-1135G7) 2.40GHz 16GB 512GB NoOPT 32MB BkLIT W10P64</t>
+  </si>
+  <si>
+    <t>dell-optiplex-3070-mff-000162</t>
+  </si>
+  <si>
+    <t>OPT 3070 MFF STD 1x i3Q (i3-9100T) 3.10GHz 16GB 500GB NoOPT 32MB  W10P64</t>
+  </si>
+  <si>
+    <t>dell-optiplex-3070-mff-000165</t>
+  </si>
+  <si>
+    <t>12 GB (1x 4GB, 1x 8GB)</t>
+  </si>
+  <si>
+    <t>OPT 3070 MFF STD 1x i3Q (i3-9100T) 3.10GHz 12GB 256GB NoOPT 32MB  W10P64</t>
+  </si>
+  <si>
+    <t>dell-optiplex-3070-mff-000166</t>
+  </si>
+  <si>
+    <t>dell-optiplex-7070-sff-000278</t>
   </si>
   <si>
     <t>Dell OptiPlex 7070 SFF</t>
@@ -278,315 +554,6 @@
     <t>1x Intel Core i5-9500 (6-Core, 3.00 GHz)</t>
   </si>
   <si>
-    <t>OPT 7070 SFF STD 1x i56C (i5-9500) 3.00GHz 8GB 256GB NoOPT 32MB  W10P64</t>
-  </si>
-  <si>
-    <t>dell-latitude-7420-touch-000059</t>
-  </si>
-  <si>
-    <t>Dell Latitude 7420 Touch</t>
-  </si>
-  <si>
-    <t>1x Intel Core i5-1145G7 (4-Core, 2.60 GHz)</t>
-  </si>
-  <si>
-    <t>64-bit Windows 10 Professional</t>
-  </si>
-  <si>
-    <t>lenovo-thinkpad-e14-gen-2-no-os-000004</t>
-  </si>
-  <si>
-    <t>Lenovo ThinkPad E14 Gen 2 - No OS</t>
-  </si>
-  <si>
-    <t>1x Intel Core i7-1165G7 (4-Core, 2.80 GHz)</t>
-  </si>
-  <si>
-    <t>TKP E14 Gen 2 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i7Q (i7-1165G7) 2.80GHz 16GB 512GB NoOPT 32MB BkLIT NoOS</t>
-  </si>
-  <si>
-    <t>dell-latitude-5420-touch-000058</t>
-  </si>
-  <si>
-    <t>Dell Latitude 5420 Touch</t>
-  </si>
-  <si>
-    <t>LAT 5420 NB STD 14-in (1920 x 1080) TCH CAM 1x i7Q (i7-1185G7) 3.00GHz 16GB 512GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-optiplex-3070-mff-000164</t>
-  </si>
-  <si>
-    <t>dell-latitude-5520-touch-000026</t>
-  </si>
-  <si>
-    <t>Dell Latitude 5520 Touch</t>
-  </si>
-  <si>
-    <t>LAT 5520 NB STD 15.6-in (1920 x 1080) TCH CAM 1x i7Q (i7-1185G7) 3.00GHz 16GB 512GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-latitude-3410-000024</t>
-  </si>
-  <si>
-    <t>Dell Latitude 3410</t>
-  </si>
-  <si>
-    <t>1x Intel Core i5-10210U (4-Core, 1.60 GHz)</t>
-  </si>
-  <si>
-    <t>LAT 3410 NB STD 14-in (1366 x 768) NoTCH CAM 1x i5Q (i5-10210U) 1.60GHz 8GB 256GB NoOPT 32MB NoBkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-precision-3561-000089</t>
-  </si>
-  <si>
-    <t>Dell Precision 3561</t>
-  </si>
-  <si>
-    <t>1x Intel Core i7-11850H (8-Core, 2.50 GHz)</t>
-  </si>
-  <si>
-    <t>PRE 3561 NB STD 15.6-in (1920 x 1080) NoTCH CAM 1x i78C (i7-11850H) 2.50GHz 16GB 512GB NoOPT 4GB BkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-latitude-7420-000282</t>
-  </si>
-  <si>
-    <t>Dell Latitude 7420</t>
-  </si>
-  <si>
-    <t>LAT 7420 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i7Q (i7-1185G7) 3.00GHz 32GB 512GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-optiplex-3090-mff-000030</t>
-  </si>
-  <si>
-    <t>Dell OptiPlex 3090 MFF</t>
-  </si>
-  <si>
-    <t>1x Intel Core i3-10105T (4-Core, 3.00 GHz)</t>
-  </si>
-  <si>
-    <t>OPT 3090 MFF STD 1x i3 (i3-10105T) 3.00GHz 8GB 256GB NoOPT 32MB  W11P64</t>
-  </si>
-  <si>
-    <t>lenovo-thinkpad-t14-no-os-000013</t>
-  </si>
-  <si>
-    <t>TKP T14 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-10210U) 1.60GHz 8GB 256GB NoOPT 32MB BkLIT NoOS</t>
-  </si>
-  <si>
-    <t>lenovo-thinkpad-t14-no-os-000015</t>
-  </si>
-  <si>
-    <t>lenovo-thinkbook-14s-yoga-touch-no-os-000008</t>
-  </si>
-  <si>
-    <t>microsoft-surface-laptop-4-touch-no-os-000006</t>
-  </si>
-  <si>
-    <t>dell-optiplex-3090-mff-000034</t>
-  </si>
-  <si>
-    <t>1x Intel Core i3-10100T (4-Core, 3.00 GHz)</t>
-  </si>
-  <si>
-    <t>OPT 3090 MFF STD 1x i3Q (i3-10100T) 3.00GHz 8GB 128GB NoOPT 32MB  W11P64</t>
-  </si>
-  <si>
-    <t>lenovo-thinkcentre-m720q-mff-000003</t>
-  </si>
-  <si>
-    <t>1x Intel Core i3-8100T (4-Core, 3.10 GHz)</t>
-  </si>
-  <si>
-    <t>TKC M720Q MFF STD 1x i3Q (i3-8100T) 3.10GHz 8GB 500GB NoOPT 32MB  W10P64</t>
-  </si>
-  <si>
-    <t>dell-optiplex-3070-mff-000112</t>
-  </si>
-  <si>
-    <t>OPT 3070 MFF STD 1x i3Q (i3-9100T) 3.10GHz 8GB 256GB NoOPT 32MB  W10P64</t>
-  </si>
-  <si>
-    <t>dell-optiplex-3060-sff-000191</t>
-  </si>
-  <si>
-    <t>dell-optiplex-3070-sff-000168</t>
-  </si>
-  <si>
-    <t>Dell OptiPlex 3070 SFF</t>
-  </si>
-  <si>
-    <t>OPT 3070 SFF STD 1x i56C (i5-9500) 3.00GHz 8GB 512GB NoOPT 32MB  W10P64</t>
-  </si>
-  <si>
-    <t>dell-optiplex-3070-mff-000123</t>
-  </si>
-  <si>
-    <t>dell-optiplex-3070-sff-000241</t>
-  </si>
-  <si>
-    <t>OPT 3070 SFF STD 1x i56C (i5-9500) 3.00GHz 16GB 512GB NoOPT 32MB  W10P64</t>
-  </si>
-  <si>
-    <t>dell-latitude-5400-000493</t>
-  </si>
-  <si>
-    <t>Dell Latitude 5400</t>
-  </si>
-  <si>
-    <t>1x Intel Core i5-8365U (4-Core, 1.60 GHz)</t>
-  </si>
-  <si>
-    <t>LAT 5400 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-8365U) 1.60GHz 8GB 256GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-latitude-7400-2-in-1-touch-000081</t>
-  </si>
-  <si>
-    <t>Dell Latitude 7400 2-in-1 Touch</t>
-  </si>
-  <si>
-    <t>1x Intel Core i5-8265U (4-Core, 1.60 GHz)</t>
-  </si>
-  <si>
-    <t>LAT 7400 2-in-1 2N1 STD 1x i5Q (i5-8265U) 1.60GHz 8GB 256GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-latitude-5400-000498</t>
-  </si>
-  <si>
-    <t>dell-latitude-5490-000607</t>
-  </si>
-  <si>
-    <t>Dell Latitude 5490</t>
-  </si>
-  <si>
-    <t>1x Intel Core i5-7300U (2-Core, 2.60 GHz)</t>
-  </si>
-  <si>
-    <t>LAT 5490 NB STD 14-in (1366 x 768) NoTCH CAM 1x i5 (i5-7300U) 2.60GHz 8GB 500GB NoOPT 32MB NoBkLIT W10P64</t>
-  </si>
-  <si>
-    <t>hp-zbook-15-g7-firefly-no-os-000001</t>
-  </si>
-  <si>
-    <t>HP Zbook 15 G7 FIREFLY - No OS</t>
-  </si>
-  <si>
-    <t>ZBK 15 G7 FIREFLY NB STD 15.6-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-10210U) 1.60GHz 16GB 512GB NoOPT 32MB BkLIT NoOS</t>
-  </si>
-  <si>
-    <t>dell-latitude-5400-000510</t>
-  </si>
-  <si>
-    <t>LAT 5400 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-8265U) 1.60GHz 8GB 256GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-latitude-5310-touch-000045</t>
-  </si>
-  <si>
-    <t>32 GB (2x 16GB)</t>
-  </si>
-  <si>
-    <t>LAT 5310 NB STD 13.3-in (1920 x 1080) TCH CAM 1x i5Q (i5-10310U) 1.70GHz 32GB 256GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
-    <t>lenovo-thinkpad-t14-no-os-000010</t>
-  </si>
-  <si>
-    <t>1x Intel Core i7-10610U (4-Core, 1.80 GHz)</t>
-  </si>
-  <si>
-    <t>TKP T14 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i7Q (i7-10610U) 1.80GHz 16GB 512GB NoOPT 32MB BkLIT NoOS</t>
-  </si>
-  <si>
-    <t>dell-latitude-5490-touch-000055</t>
-  </si>
-  <si>
-    <t>Dell Latitude 5490 Touch</t>
-  </si>
-  <si>
-    <t>1x Intel Core i5-8350U (4-Core, 1.70 GHz)</t>
-  </si>
-  <si>
-    <t>LAT 5490 NB STD 14-in (1920 x 1080) TCH CAM 1x i5Q (i5-8350U) 1.70GHz 8GB 500GB NoOPT 32MB NoBkLIT W10P64</t>
-  </si>
-  <si>
-    <t>lenovo-thinkpad-t14-no-os-000012</t>
-  </si>
-  <si>
-    <t>dell-latitude-5420-000420</t>
-  </si>
-  <si>
-    <t>Dell Latitude 5420</t>
-  </si>
-  <si>
-    <t>LAT 5420 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-1135G7) 2.40GHz 8GB 256GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-latitude-5420-000431</t>
-  </si>
-  <si>
-    <t>LAT 5420 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i7Q (i7-1185G7) 3.00GHz 32GB 512GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-latitude-5410-000457</t>
-  </si>
-  <si>
-    <t>LAT 5410 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-10310U) 1.70GHz 16GB 256GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-latitude-5420-000440</t>
-  </si>
-  <si>
-    <t>LAT 5420 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-1145G7) 2.60GHz 16GB 512GB NoOPT 32MB NoBkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-optiplex-3080-sff-000144</t>
-  </si>
-  <si>
-    <t>Dell OptiPlex 3080 SFF</t>
-  </si>
-  <si>
-    <t>1x Intel Celeron G5900 (2-Core, 3.40 GHz)</t>
-  </si>
-  <si>
-    <t>24 GB (1x 8GB, 1x 16GB)</t>
-  </si>
-  <si>
-    <t>OPT 3080 SFF STD 1x CDC (G5900) 3.40GHz 24GB 256GB NoOPT 32MB  W10P64</t>
-  </si>
-  <si>
-    <t>dell-latitude-3420-000030</t>
-  </si>
-  <si>
-    <t>LAT 3420 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-1135G7) 2.40GHz 16GB 512GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-optiplex-3070-mff-000162</t>
-  </si>
-  <si>
-    <t>OPT 3070 MFF STD 1x i3Q (i3-9100T) 3.10GHz 16GB 500GB NoOPT 32MB  W10P64</t>
-  </si>
-  <si>
-    <t>dell-optiplex-3070-mff-000165</t>
-  </si>
-  <si>
-    <t>12 GB (1x 4GB, 1x 8GB)</t>
-  </si>
-  <si>
-    <t>OPT 3070 MFF STD 1x i3Q (i3-9100T) 3.10GHz 12GB 256GB NoOPT 32MB  W10P64</t>
-  </si>
-  <si>
-    <t>dell-optiplex-3070-mff-000166</t>
-  </si>
-  <si>
-    <t>dell-optiplex-7070-sff-000278</t>
-  </si>
-  <si>
     <t>OPT 7070 SFF STD 1x i56C (i5-9500) 3.00GHz 8GB 128GB NoOPT 32MB  W10P64</t>
   </si>
   <si>
@@ -969,12 +936,6 @@
   </si>
   <si>
     <t>dell-optiplex-3080-sff-000161</t>
-  </si>
-  <si>
-    <t>dell-optiplex-7070-sff-000284</t>
-  </si>
-  <si>
-    <t>OPT 7070 SFF STD 1x i56C (i5-9500) 3.00GHz 16GB 256GB NoOPT 32MB  W10P64</t>
   </si>
   <si>
     <t>microsoft-suface-book-3-touch-no-os-000001</t>
@@ -1530,7 +1491,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H139"/>
+  <dimension ref="A1:H134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1835,16 +1796,16 @@
         <v>3</v>
       </c>
       <c r="D12">
-        <v>282.0</v>
+        <v>386.0</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
         <v>55</v>
@@ -1861,16 +1822,16 @@
         <v>3</v>
       </c>
       <c r="D13">
-        <v>386.0</v>
+        <v>219.0</v>
       </c>
       <c r="E13" t="s">
         <v>58</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H13" t="s">
         <v>59</v>
@@ -1887,16 +1848,16 @@
         <v>3</v>
       </c>
       <c r="D14">
-        <v>219.0</v>
+        <v>516.0</v>
       </c>
       <c r="E14" t="s">
         <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H14" t="s">
         <v>63</v>
@@ -1913,16 +1874,16 @@
         <v>3</v>
       </c>
       <c r="D15">
-        <v>516.0</v>
+        <v>458.0</v>
       </c>
       <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
         <v>66</v>
-      </c>
-      <c r="F15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" t="s">
-        <v>20</v>
       </c>
       <c r="H15" t="s">
         <v>67</v>
@@ -1939,36 +1900,36 @@
         <v>3</v>
       </c>
       <c r="D16">
-        <v>458.0</v>
+        <v>901.0</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" t="s">
         <v>70</v>
-      </c>
-      <c r="H16" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
         <v>72</v>
-      </c>
-      <c r="B17" t="s">
-        <v>73</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
       <c r="D17">
-        <v>901.0</v>
+        <v>456.0</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
         <v>31</v>
@@ -1991,36 +1952,36 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <v>456.0</v>
+        <v>416.0</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
         <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>416.0</v>
+        <v>202.0</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="F19" t="s">
         <v>11</v>
@@ -2029,33 +1990,30 @@
         <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20">
-        <v>202.0</v>
+        <v>669.0</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="G20" t="s">
         <v>20</v>
-      </c>
-      <c r="H20" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2069,16 +2027,16 @@
         <v>2</v>
       </c>
       <c r="D21">
-        <v>299.0</v>
+        <v>466.0</v>
       </c>
       <c r="E21" t="s">
         <v>86</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H21" t="s">
         <v>87</v>
@@ -2095,59 +2053,62 @@
         <v>2</v>
       </c>
       <c r="D22">
-        <v>669.0</v>
+        <v>425.0</v>
       </c>
       <c r="E22" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="F22" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="G22" t="s">
         <v>20</v>
       </c>
+      <c r="H22" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23">
-        <v>466.0</v>
+        <v>198.0</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G23" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24">
-        <v>425.0</v>
+        <v>448.0</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F24" t="s">
         <v>11</v>
@@ -2156,24 +2117,24 @@
         <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
       <c r="D25">
-        <v>198.0</v>
+        <v>256.0</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>97</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
@@ -2182,24 +2143,24 @@
         <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" t="s">
         <v>100</v>
-      </c>
-      <c r="B26" t="s">
-        <v>101</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26">
-        <v>448.0</v>
+        <v>902.0</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="F26" t="s">
         <v>11</v>
@@ -2222,114 +2183,114 @@
         <v>2</v>
       </c>
       <c r="D27">
-        <v>256.0</v>
+        <v>490.0</v>
       </c>
       <c r="E27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" t="s">
         <v>105</v>
-      </c>
-      <c r="F27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" t="s">
         <v>107</v>
-      </c>
-      <c r="B28" t="s">
-        <v>108</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28">
-        <v>902.0</v>
+        <v>345.0</v>
       </c>
       <c r="E28" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
         <v>109</v>
-      </c>
-      <c r="F28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29">
-        <v>490.0</v>
+        <v>291.0</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G29" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30">
-        <v>345.0</v>
+        <v>456.0</v>
       </c>
       <c r="E30" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="F30" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G30" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>117</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31">
-        <v>291.0</v>
+        <v>386.0</v>
       </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="F31" t="s">
         <v>31</v>
@@ -2338,24 +2299,24 @@
         <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32">
-        <v>456.0</v>
+        <v>901.0</v>
       </c>
       <c r="E32" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="F32" t="s">
         <v>31</v>
@@ -2364,116 +2325,116 @@
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33">
-        <v>386.0</v>
+        <v>334.0</v>
       </c>
       <c r="E33" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="F33" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G33" t="s">
         <v>12</v>
       </c>
       <c r="H33" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34">
-        <v>901.0</v>
+        <v>160.0</v>
       </c>
       <c r="E34" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
       <c r="F34" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G34" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>115</v>
+        <v>15</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35">
-        <v>334.0</v>
+        <v>199.0</v>
       </c>
       <c r="E35" t="s">
-        <v>124</v>
+        <v>16</v>
       </c>
       <c r="F35" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="G35" t="s">
         <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36">
-        <v>160.0</v>
+        <v>202.0</v>
       </c>
       <c r="E36" t="s">
-        <v>127</v>
+        <v>46</v>
       </c>
       <c r="F36" t="s">
         <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H36" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
@@ -2494,76 +2455,76 @@
         <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38">
-        <v>202.0</v>
+        <v>142.0</v>
       </c>
       <c r="E38" t="s">
-        <v>46</v>
+        <v>127</v>
       </c>
       <c r="F38" t="s">
         <v>11</v>
       </c>
       <c r="G38" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H38" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>246.0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" t="s">
         <v>132</v>
-      </c>
-      <c r="B39" t="s">
-        <v>133</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>256.0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>86</v>
-      </c>
-      <c r="F39" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40">
-        <v>199.0</v>
+        <v>142.0</v>
       </c>
       <c r="E40" t="s">
-        <v>16</v>
+        <v>127</v>
       </c>
       <c r="F40" t="s">
         <v>11</v>
@@ -2572,30 +2533,30 @@
         <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>80.0</v>
+      </c>
+      <c r="E41" t="s">
         <v>136</v>
       </c>
-      <c r="B41" t="s">
-        <v>133</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>276.0</v>
-      </c>
-      <c r="E41" t="s">
-        <v>86</v>
-      </c>
       <c r="F41" t="s">
         <v>11</v>
       </c>
       <c r="G41" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H41" t="s">
         <v>137</v>
@@ -2612,322 +2573,322 @@
         <v>1</v>
       </c>
       <c r="D42">
-        <v>142.0</v>
+        <v>271.0</v>
       </c>
       <c r="E42" t="s">
+        <v>97</v>
+      </c>
+      <c r="F42" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" t="s">
         <v>140</v>
-      </c>
-      <c r="F42" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>142.0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>131</v>
+      </c>
+      <c r="F43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" t="s">
         <v>142</v>
-      </c>
-      <c r="B43" t="s">
-        <v>143</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43">
-        <v>246.0</v>
-      </c>
-      <c r="E43" t="s">
-        <v>144</v>
-      </c>
-      <c r="F43" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H43" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B44" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44">
-        <v>142.0</v>
+        <v>352.0</v>
       </c>
       <c r="E44" t="s">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="F44" t="s">
         <v>11</v>
       </c>
       <c r="G44" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="H44" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
+        <v>146</v>
+      </c>
+      <c r="B45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>396.0</v>
+      </c>
+      <c r="E45" t="s">
         <v>147</v>
       </c>
-      <c r="B45" t="s">
+      <c r="F45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G45" t="s">
+        <v>20</v>
+      </c>
+      <c r="H45" t="s">
         <v>148</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>80.0</v>
-      </c>
-      <c r="E45" t="s">
-        <v>149</v>
-      </c>
-      <c r="F45" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" t="s">
-        <v>12</v>
-      </c>
-      <c r="H45" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
+        <v>149</v>
+      </c>
+      <c r="B46" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>155.0</v>
+      </c>
+      <c r="E46" t="s">
         <v>151</v>
       </c>
-      <c r="B46" t="s">
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" t="s">
         <v>152</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>271.0</v>
-      </c>
-      <c r="E46" t="s">
-        <v>105</v>
-      </c>
-      <c r="F46" t="s">
-        <v>31</v>
-      </c>
-      <c r="G46" t="s">
-        <v>32</v>
-      </c>
-      <c r="H46" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B47" t="s">
-        <v>139</v>
+        <v>72</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>142.0</v>
+        <v>291.0</v>
       </c>
       <c r="E47" t="s">
-        <v>144</v>
+        <v>97</v>
       </c>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G47" t="s">
         <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" t="s">
+        <v>155</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>305.0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>54</v>
+      </c>
+      <c r="F48" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" t="s">
         <v>156</v>
-      </c>
-      <c r="B48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="D48">
-        <v>352.0</v>
-      </c>
-      <c r="E48" t="s">
-        <v>10</v>
-      </c>
-      <c r="F48" t="s">
-        <v>11</v>
-      </c>
-      <c r="G48" t="s">
-        <v>157</v>
-      </c>
-      <c r="H48" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B49" t="s">
-        <v>76</v>
+        <v>155</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>396.0</v>
+        <v>435.0</v>
       </c>
       <c r="E49" t="s">
-        <v>160</v>
+        <v>62</v>
       </c>
       <c r="F49" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G49" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="H49" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B50" t="s">
-        <v>163</v>
+        <v>9</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <v>155.0</v>
+        <v>249.0</v>
       </c>
       <c r="E50" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="F50" t="s">
         <v>11</v>
       </c>
       <c r="G50" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H50" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B51" t="s">
-        <v>76</v>
+        <v>155</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>291.0</v>
+        <v>335.0</v>
       </c>
       <c r="E51" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="F51" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G51" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H51" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>230.0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>165</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" t="s">
+        <v>166</v>
+      </c>
+      <c r="H52" t="s">
         <v>167</v>
-      </c>
-      <c r="B52" t="s">
-        <v>168</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>305.0</v>
-      </c>
-      <c r="E52" t="s">
-        <v>58</v>
-      </c>
-      <c r="F52" t="s">
-        <v>11</v>
-      </c>
-      <c r="G52" t="s">
-        <v>12</v>
-      </c>
-      <c r="H52" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B53" t="s">
-        <v>168</v>
+        <v>35</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53">
-        <v>435.0</v>
+        <v>386.0</v>
       </c>
       <c r="E53" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="F53" t="s">
         <v>11</v>
       </c>
       <c r="G53" t="s">
-        <v>157</v>
+        <v>32</v>
       </c>
       <c r="H53" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54">
-        <v>249.0</v>
+        <v>218.0</v>
       </c>
       <c r="E54" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F54" t="s">
         <v>11</v>
@@ -2936,90 +2897,90 @@
         <v>32</v>
       </c>
       <c r="H54" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
+        <v>172</v>
+      </c>
+      <c r="B55" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>209.0</v>
+      </c>
+      <c r="E55" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" t="s">
+        <v>173</v>
+      </c>
+      <c r="H55" t="s">
         <v>174</v>
-      </c>
-      <c r="B55" t="s">
-        <v>168</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55">
-        <v>335.0</v>
-      </c>
-      <c r="E55" t="s">
-        <v>90</v>
-      </c>
-      <c r="F55" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" t="s">
-        <v>20</v>
-      </c>
-      <c r="H55" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B56" t="s">
-        <v>177</v>
+        <v>15</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56">
-        <v>230.0</v>
+        <v>199.0</v>
       </c>
       <c r="E56" t="s">
-        <v>178</v>
+        <v>16</v>
       </c>
       <c r="F56" t="s">
         <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>179</v>
+        <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>180</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B57" t="s">
-        <v>35</v>
+        <v>177</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57">
-        <v>386.0</v>
+        <v>288.0</v>
       </c>
       <c r="E57" t="s">
-        <v>58</v>
+        <v>178</v>
       </c>
       <c r="F57" t="s">
         <v>11</v>
       </c>
       <c r="G57" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H57" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B58" t="s">
         <v>15</v>
@@ -3028,7 +2989,7 @@
         <v>1</v>
       </c>
       <c r="D58">
-        <v>218.0</v>
+        <v>219.0</v>
       </c>
       <c r="E58" t="s">
         <v>16</v>
@@ -3037,15 +2998,15 @@
         <v>11</v>
       </c>
       <c r="G58" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H58" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B59" t="s">
         <v>15</v>
@@ -3054,7 +3015,7 @@
         <v>1</v>
       </c>
       <c r="D59">
-        <v>209.0</v>
+        <v>219.0</v>
       </c>
       <c r="E59" t="s">
         <v>16</v>
@@ -3063,215 +3024,215 @@
         <v>11</v>
       </c>
       <c r="G59" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="H59" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B60" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60">
-        <v>199.0</v>
+        <v>352.0</v>
       </c>
       <c r="E60" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F60" t="s">
         <v>11</v>
       </c>
       <c r="G60" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="H60" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B61" t="s">
-        <v>85</v>
+        <v>186</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61">
-        <v>288.0</v>
+        <v>475.0</v>
       </c>
       <c r="E61" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="F61" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G61" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="H61" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>189</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62">
-        <v>219.0</v>
+        <v>425.0</v>
       </c>
       <c r="E62" t="s">
-        <v>16</v>
+        <v>147</v>
       </c>
       <c r="F62" t="s">
         <v>11</v>
       </c>
       <c r="G62" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H62" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>401.0</v>
+      </c>
+      <c r="E63" t="s">
         <v>193</v>
       </c>
-      <c r="B63" t="s">
-        <v>15</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63">
-        <v>219.0</v>
-      </c>
-      <c r="E63" t="s">
-        <v>16</v>
-      </c>
       <c r="F63" t="s">
         <v>11</v>
       </c>
       <c r="G63" t="s">
-        <v>12</v>
+        <v>194</v>
       </c>
       <c r="H63" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B64" t="s">
-        <v>19</v>
+        <v>197</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64">
-        <v>352.0</v>
+        <v>261.0</v>
       </c>
       <c r="E64" t="s">
-        <v>10</v>
+        <v>127</v>
       </c>
       <c r="F64" t="s">
         <v>11</v>
       </c>
       <c r="G64" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="H64" t="s">
-        <v>158</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B65" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65">
-        <v>475.0</v>
+        <v>249.0</v>
       </c>
       <c r="E65" t="s">
-        <v>109</v>
+        <v>165</v>
       </c>
       <c r="F65" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G65" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="H65" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B66" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66">
-        <v>425.0</v>
+        <v>189.0</v>
       </c>
       <c r="E66" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="F66" t="s">
         <v>11</v>
       </c>
       <c r="G66" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H66" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B67" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67">
-        <v>401.0</v>
+        <v>253.0</v>
       </c>
       <c r="E67" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F67" t="s">
         <v>11</v>
       </c>
       <c r="G67" t="s">
-        <v>205</v>
+        <v>32</v>
       </c>
       <c r="H67" t="s">
         <v>206</v>
@@ -3288,10 +3249,10 @@
         <v>1</v>
       </c>
       <c r="D68">
-        <v>261.0</v>
+        <v>348.0</v>
       </c>
       <c r="E68" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="F68" t="s">
         <v>11</v>
@@ -3308,7 +3269,7 @@
         <v>210</v>
       </c>
       <c r="B69" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -3317,13 +3278,13 @@
         <v>249.0</v>
       </c>
       <c r="E69" t="s">
-        <v>178</v>
+        <v>97</v>
       </c>
       <c r="F69" t="s">
         <v>11</v>
       </c>
       <c r="G69" t="s">
-        <v>157</v>
+        <v>32</v>
       </c>
       <c r="H69" t="s">
         <v>211</v>
@@ -3334,22 +3295,22 @@
         <v>212</v>
       </c>
       <c r="B70" t="s">
-        <v>177</v>
+        <v>104</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70">
-        <v>189.0</v>
+        <v>520.0</v>
       </c>
       <c r="E70" t="s">
-        <v>178</v>
+        <v>62</v>
       </c>
       <c r="F70" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G70" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="H70" t="s">
         <v>213</v>
@@ -3360,308 +3321,308 @@
         <v>214</v>
       </c>
       <c r="B71" t="s">
+        <v>192</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>421.0</v>
+      </c>
+      <c r="E71" t="s">
         <v>215</v>
       </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
-      <c r="D71">
-        <v>253.0</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
+        <v>37</v>
+      </c>
+      <c r="G71" t="s">
+        <v>194</v>
+      </c>
+      <c r="H71" t="s">
         <v>216</v>
-      </c>
-      <c r="F71" t="s">
-        <v>11</v>
-      </c>
-      <c r="G71" t="s">
-        <v>32</v>
-      </c>
-      <c r="H71" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
+        <v>217</v>
+      </c>
+      <c r="B72" t="s">
         <v>218</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>619.0</v>
+      </c>
+      <c r="E72" t="s">
+        <v>101</v>
+      </c>
+      <c r="F72" t="s">
+        <v>11</v>
+      </c>
+      <c r="G72" t="s">
+        <v>144</v>
+      </c>
+      <c r="H72" t="s">
         <v>219</v>
-      </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-      <c r="D72">
-        <v>348.0</v>
-      </c>
-      <c r="E72" t="s">
-        <v>90</v>
-      </c>
-      <c r="F72" t="s">
-        <v>11</v>
-      </c>
-      <c r="G72" t="s">
-        <v>32</v>
-      </c>
-      <c r="H72" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
+        <v>220</v>
+      </c>
+      <c r="B73" t="s">
+        <v>208</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>328.0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>82</v>
+      </c>
+      <c r="F73" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73" t="s">
         <v>221</v>
-      </c>
-      <c r="B73" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
-      <c r="D73">
-        <v>249.0</v>
-      </c>
-      <c r="E73" t="s">
-        <v>105</v>
-      </c>
-      <c r="F73" t="s">
-        <v>11</v>
-      </c>
-      <c r="G73" t="s">
-        <v>32</v>
-      </c>
-      <c r="H73" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
+        <v>222</v>
+      </c>
+      <c r="B74" t="s">
+        <v>155</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>395.0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>86</v>
+      </c>
+      <c r="F74" t="s">
+        <v>11</v>
+      </c>
+      <c r="G74" t="s">
+        <v>20</v>
+      </c>
+      <c r="H74" t="s">
         <v>223</v>
-      </c>
-      <c r="B74" t="s">
-        <v>112</v>
-      </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
-      <c r="D74">
-        <v>520.0</v>
-      </c>
-      <c r="E74" t="s">
-        <v>66</v>
-      </c>
-      <c r="F74" t="s">
-        <v>37</v>
-      </c>
-      <c r="G74" t="s">
-        <v>70</v>
-      </c>
-      <c r="H74" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
+        <v>224</v>
+      </c>
+      <c r="B75" t="s">
         <v>225</v>
       </c>
-      <c r="B75" t="s">
-        <v>203</v>
-      </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75">
-        <v>421.0</v>
+        <v>419.0</v>
       </c>
       <c r="E75" t="s">
+        <v>147</v>
+      </c>
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75" t="s">
+        <v>20</v>
+      </c>
+      <c r="H75" t="s">
         <v>226</v>
-      </c>
-      <c r="F75" t="s">
-        <v>37</v>
-      </c>
-      <c r="G75" t="s">
-        <v>205</v>
-      </c>
-      <c r="H75" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
+        <v>227</v>
+      </c>
+      <c r="B76" t="s">
         <v>228</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>416.0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>147</v>
+      </c>
+      <c r="F76" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76" t="s">
+        <v>32</v>
+      </c>
+      <c r="H76" t="s">
         <v>229</v>
-      </c>
-      <c r="C76">
-        <v>1</v>
-      </c>
-      <c r="D76">
-        <v>619.0</v>
-      </c>
-      <c r="E76" t="s">
-        <v>109</v>
-      </c>
-      <c r="F76" t="s">
-        <v>11</v>
-      </c>
-      <c r="G76" t="s">
-        <v>157</v>
-      </c>
-      <c r="H76" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
+        <v>230</v>
+      </c>
+      <c r="B77" t="s">
+        <v>65</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>368.0</v>
+      </c>
+      <c r="E77" t="s">
+        <v>82</v>
+      </c>
+      <c r="F77" t="s">
+        <v>11</v>
+      </c>
+      <c r="G77" t="s">
+        <v>20</v>
+      </c>
+      <c r="H77" t="s">
         <v>231</v>
-      </c>
-      <c r="B77" t="s">
-        <v>219</v>
-      </c>
-      <c r="C77">
-        <v>1</v>
-      </c>
-      <c r="D77">
-        <v>328.0</v>
-      </c>
-      <c r="E77" t="s">
-        <v>90</v>
-      </c>
-      <c r="F77" t="s">
-        <v>11</v>
-      </c>
-      <c r="G77" t="s">
-        <v>12</v>
-      </c>
-      <c r="H77" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
+        <v>232</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>219.0</v>
+      </c>
+      <c r="E78" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" t="s">
+        <v>11</v>
+      </c>
+      <c r="G78" t="s">
+        <v>12</v>
+      </c>
+      <c r="H78" t="s">
         <v>233</v>
-      </c>
-      <c r="B78" t="s">
-        <v>168</v>
-      </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-      <c r="D78">
-        <v>395.0</v>
-      </c>
-      <c r="E78" t="s">
-        <v>94</v>
-      </c>
-      <c r="F78" t="s">
-        <v>11</v>
-      </c>
-      <c r="G78" t="s">
-        <v>20</v>
-      </c>
-      <c r="H78" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
+        <v>234</v>
+      </c>
+      <c r="B79" t="s">
         <v>235</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>566.0</v>
+      </c>
+      <c r="E79" t="s">
+        <v>101</v>
+      </c>
+      <c r="F79" t="s">
+        <v>11</v>
+      </c>
+      <c r="G79" t="s">
+        <v>32</v>
+      </c>
+      <c r="H79" t="s">
         <v>236</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
-      </c>
-      <c r="D79">
-        <v>419.0</v>
-      </c>
-      <c r="E79" t="s">
-        <v>160</v>
-      </c>
-      <c r="F79" t="s">
-        <v>11</v>
-      </c>
-      <c r="G79" t="s">
-        <v>20</v>
-      </c>
-      <c r="H79" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
+        <v>237</v>
+      </c>
+      <c r="B80" t="s">
+        <v>96</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>211.0</v>
+      </c>
+      <c r="E80" t="s">
         <v>238</v>
       </c>
-      <c r="B80" t="s">
+      <c r="F80" t="s">
+        <v>11</v>
+      </c>
+      <c r="G80" t="s">
+        <v>12</v>
+      </c>
+      <c r="H80" t="s">
         <v>239</v>
-      </c>
-      <c r="C80">
-        <v>1</v>
-      </c>
-      <c r="D80">
-        <v>416.0</v>
-      </c>
-      <c r="E80" t="s">
-        <v>160</v>
-      </c>
-      <c r="F80" t="s">
-        <v>11</v>
-      </c>
-      <c r="G80" t="s">
-        <v>32</v>
-      </c>
-      <c r="H80" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
+        <v>240</v>
+      </c>
+      <c r="B81" t="s">
+        <v>218</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>520.0</v>
+      </c>
+      <c r="E81" t="s">
+        <v>101</v>
+      </c>
+      <c r="F81" t="s">
+        <v>11</v>
+      </c>
+      <c r="G81" t="s">
+        <v>32</v>
+      </c>
+      <c r="H81" t="s">
         <v>241</v>
-      </c>
-      <c r="B81" t="s">
-        <v>69</v>
-      </c>
-      <c r="C81">
-        <v>1</v>
-      </c>
-      <c r="D81">
-        <v>368.0</v>
-      </c>
-      <c r="E81" t="s">
-        <v>90</v>
-      </c>
-      <c r="F81" t="s">
-        <v>11</v>
-      </c>
-      <c r="G81" t="s">
-        <v>20</v>
-      </c>
-      <c r="H81" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
+        <v>242</v>
+      </c>
+      <c r="B82" t="s">
         <v>243</v>
       </c>
-      <c r="B82" t="s">
-        <v>9</v>
-      </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82">
-        <v>219.0</v>
+        <v>418.0</v>
       </c>
       <c r="E82" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="F82" t="s">
         <v>11</v>
       </c>
       <c r="G82" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="H82" t="s">
         <v>244</v>
@@ -3672,42 +3633,42 @@
         <v>245</v>
       </c>
       <c r="B83" t="s">
+        <v>81</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>530.0</v>
+      </c>
+      <c r="E83" t="s">
+        <v>62</v>
+      </c>
+      <c r="F83" t="s">
+        <v>37</v>
+      </c>
+      <c r="G83" t="s">
+        <v>20</v>
+      </c>
+      <c r="H83" t="s">
         <v>246</v>
-      </c>
-      <c r="C83">
-        <v>1</v>
-      </c>
-      <c r="D83">
-        <v>566.0</v>
-      </c>
-      <c r="E83" t="s">
-        <v>109</v>
-      </c>
-      <c r="F83" t="s">
-        <v>11</v>
-      </c>
-      <c r="G83" t="s">
-        <v>32</v>
-      </c>
-      <c r="H83" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
+        <v>247</v>
+      </c>
+      <c r="B84" t="s">
         <v>248</v>
       </c>
-      <c r="B84" t="s">
-        <v>104</v>
-      </c>
       <c r="C84">
         <v>1</v>
       </c>
       <c r="D84">
-        <v>211.0</v>
+        <v>248.0</v>
       </c>
       <c r="E84" t="s">
-        <v>249</v>
+        <v>10</v>
       </c>
       <c r="F84" t="s">
         <v>11</v>
@@ -3716,56 +3677,56 @@
         <v>12</v>
       </c>
       <c r="H84" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
+        <v>250</v>
+      </c>
+      <c r="B85" t="s">
+        <v>208</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>328.0</v>
+      </c>
+      <c r="E85" t="s">
+        <v>54</v>
+      </c>
+      <c r="F85" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" t="s">
+        <v>12</v>
+      </c>
+      <c r="H85" t="s">
         <v>251</v>
-      </c>
-      <c r="B85" t="s">
-        <v>229</v>
-      </c>
-      <c r="C85">
-        <v>1</v>
-      </c>
-      <c r="D85">
-        <v>520.0</v>
-      </c>
-      <c r="E85" t="s">
-        <v>109</v>
-      </c>
-      <c r="F85" t="s">
-        <v>11</v>
-      </c>
-      <c r="G85" t="s">
-        <v>32</v>
-      </c>
-      <c r="H85" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
+        <v>252</v>
+      </c>
+      <c r="B86" t="s">
         <v>253</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>120.0</v>
+      </c>
+      <c r="E86" t="s">
         <v>254</v>
       </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-      <c r="D86">
-        <v>418.0</v>
-      </c>
-      <c r="E86" t="s">
-        <v>66</v>
-      </c>
       <c r="F86" t="s">
         <v>11</v>
       </c>
       <c r="G86" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="H86" t="s">
         <v>255</v>
@@ -3776,22 +3737,22 @@
         <v>256</v>
       </c>
       <c r="B87" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="C87">
         <v>1</v>
       </c>
       <c r="D87">
-        <v>530.0</v>
+        <v>811.0</v>
       </c>
       <c r="E87" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="F87" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G87" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H87" t="s">
         <v>257</v>
@@ -3802,13 +3763,13 @@
         <v>258</v>
       </c>
       <c r="B88" t="s">
-        <v>259</v>
+        <v>9</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
       <c r="D88">
-        <v>248.0</v>
+        <v>219.0</v>
       </c>
       <c r="E88" t="s">
         <v>10</v>
@@ -3817,85 +3778,85 @@
         <v>11</v>
       </c>
       <c r="G88" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H88" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
+        <v>260</v>
+      </c>
+      <c r="B89" t="s">
+        <v>72</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>436.0</v>
+      </c>
+      <c r="E89" t="s">
+        <v>147</v>
+      </c>
+      <c r="F89" t="s">
+        <v>31</v>
+      </c>
+      <c r="G89" t="s">
+        <v>144</v>
+      </c>
+      <c r="H89" t="s">
         <v>261</v>
-      </c>
-      <c r="B89" t="s">
-        <v>219</v>
-      </c>
-      <c r="C89">
-        <v>1</v>
-      </c>
-      <c r="D89">
-        <v>328.0</v>
-      </c>
-      <c r="E89" t="s">
-        <v>58</v>
-      </c>
-      <c r="F89" t="s">
-        <v>11</v>
-      </c>
-      <c r="G89" t="s">
-        <v>12</v>
-      </c>
-      <c r="H89" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
+        <v>262</v>
+      </c>
+      <c r="B90" t="s">
         <v>263</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>336.0</v>
+      </c>
+      <c r="E90" t="s">
+        <v>147</v>
+      </c>
+      <c r="F90" t="s">
+        <v>31</v>
+      </c>
+      <c r="G90" t="s">
+        <v>32</v>
+      </c>
+      <c r="H90" t="s">
         <v>264</v>
-      </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-      <c r="D90">
-        <v>120.0</v>
-      </c>
-      <c r="E90" t="s">
-        <v>265</v>
-      </c>
-      <c r="F90" t="s">
-        <v>11</v>
-      </c>
-      <c r="G90" t="s">
-        <v>42</v>
-      </c>
-      <c r="H90" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="91" spans="1:8">
       <c r="A91" t="s">
+        <v>265</v>
+      </c>
+      <c r="B91" t="s">
+        <v>266</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>525.0</v>
+      </c>
+      <c r="E91" t="s">
         <v>267</v>
-      </c>
-      <c r="B91" t="s">
-        <v>73</v>
-      </c>
-      <c r="C91">
-        <v>1</v>
-      </c>
-      <c r="D91">
-        <v>811.0</v>
-      </c>
-      <c r="E91" t="s">
-        <v>90</v>
       </c>
       <c r="F91" t="s">
         <v>31</v>
       </c>
       <c r="G91" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="H91" t="s">
         <v>268</v>
@@ -3906,74 +3867,74 @@
         <v>269</v>
       </c>
       <c r="B92" t="s">
-        <v>9</v>
+        <v>270</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
       <c r="D92">
-        <v>219.0</v>
+        <v>691.0</v>
       </c>
       <c r="E92" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="F92" t="s">
         <v>11</v>
       </c>
       <c r="G92" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="H92" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B93" t="s">
-        <v>76</v>
+        <v>225</v>
       </c>
       <c r="C93">
         <v>1</v>
       </c>
       <c r="D93">
-        <v>436.0</v>
+        <v>314.0</v>
       </c>
       <c r="E93" t="s">
-        <v>160</v>
+        <v>10</v>
       </c>
       <c r="F93" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G93" t="s">
-        <v>157</v>
+        <v>12</v>
       </c>
       <c r="H93" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="94" spans="1:8">
       <c r="A94" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B94" t="s">
-        <v>274</v>
+        <v>208</v>
       </c>
       <c r="C94">
         <v>1</v>
       </c>
       <c r="D94">
-        <v>336.0</v>
+        <v>418.0</v>
       </c>
       <c r="E94" t="s">
-        <v>160</v>
+        <v>62</v>
       </c>
       <c r="F94" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G94" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H94" t="s">
         <v>275</v>
@@ -3984,100 +3945,100 @@
         <v>276</v>
       </c>
       <c r="B95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>214.0</v>
+      </c>
+      <c r="E95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F95" t="s">
+        <v>11</v>
+      </c>
+      <c r="G95" t="s">
+        <v>12</v>
+      </c>
+      <c r="H95" t="s">
         <v>277</v>
-      </c>
-      <c r="C95">
-        <v>1</v>
-      </c>
-      <c r="D95">
-        <v>525.0</v>
-      </c>
-      <c r="E95" t="s">
-        <v>278</v>
-      </c>
-      <c r="F95" t="s">
-        <v>31</v>
-      </c>
-      <c r="G95" t="s">
-        <v>70</v>
-      </c>
-      <c r="H95" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B96" t="s">
-        <v>281</v>
+        <v>81</v>
       </c>
       <c r="C96">
         <v>1</v>
       </c>
       <c r="D96">
-        <v>691.0</v>
+        <v>460.0</v>
       </c>
       <c r="E96" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="F96" t="s">
         <v>11</v>
       </c>
       <c r="G96" t="s">
-        <v>205</v>
+        <v>20</v>
       </c>
       <c r="H96" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B97" t="s">
-        <v>236</v>
+        <v>96</v>
       </c>
       <c r="C97">
         <v>1</v>
       </c>
       <c r="D97">
-        <v>314.0</v>
+        <v>301.0</v>
       </c>
       <c r="E97" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="F97" t="s">
-        <v>11</v>
+        <v>281</v>
       </c>
       <c r="G97" t="s">
         <v>12</v>
       </c>
       <c r="H97" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
+        <v>283</v>
+      </c>
+      <c r="B98" t="s">
+        <v>284</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>455.0</v>
+      </c>
+      <c r="E98" t="s">
         <v>285</v>
       </c>
-      <c r="B98" t="s">
-        <v>219</v>
-      </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
-      <c r="D98">
-        <v>418.0</v>
-      </c>
-      <c r="E98" t="s">
-        <v>66</v>
-      </c>
       <c r="F98" t="s">
         <v>11</v>
       </c>
       <c r="G98" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H98" t="s">
         <v>286</v>
@@ -4088,126 +4049,126 @@
         <v>287</v>
       </c>
       <c r="B99" t="s">
-        <v>9</v>
+        <v>288</v>
       </c>
       <c r="C99">
         <v>1</v>
       </c>
       <c r="D99">
-        <v>214.0</v>
+        <v>1134.0</v>
       </c>
       <c r="E99" t="s">
-        <v>10</v>
+        <v>289</v>
       </c>
       <c r="F99" t="s">
         <v>11</v>
       </c>
       <c r="G99" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="H99" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B100" t="s">
-        <v>89</v>
+        <v>292</v>
       </c>
       <c r="C100">
         <v>1</v>
       </c>
       <c r="D100">
-        <v>460.0</v>
+        <v>409.0</v>
       </c>
       <c r="E100" t="s">
-        <v>66</v>
+        <v>293</v>
       </c>
       <c r="F100" t="s">
         <v>11</v>
       </c>
       <c r="G100" t="s">
-        <v>20</v>
+        <v>294</v>
       </c>
       <c r="H100" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
     </row>
     <row r="101" spans="1:8">
       <c r="A101" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="B101" t="s">
-        <v>104</v>
+        <v>248</v>
       </c>
       <c r="C101">
         <v>1</v>
       </c>
       <c r="D101">
-        <v>301.0</v>
+        <v>303.0</v>
       </c>
       <c r="E101" t="s">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="F101" t="s">
-        <v>292</v>
+        <v>11</v>
       </c>
       <c r="G101" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H101" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B102" t="s">
-        <v>295</v>
+        <v>76</v>
       </c>
       <c r="C102">
         <v>1</v>
       </c>
       <c r="D102">
-        <v>455.0</v>
+        <v>416.0</v>
       </c>
       <c r="E102" t="s">
-        <v>296</v>
+        <v>54</v>
       </c>
       <c r="F102" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G102" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H102" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B103" t="s">
-        <v>299</v>
+        <v>164</v>
       </c>
       <c r="C103">
         <v>1</v>
       </c>
       <c r="D103">
-        <v>1134.0</v>
+        <v>239.0</v>
       </c>
       <c r="E103" t="s">
-        <v>300</v>
+        <v>165</v>
       </c>
       <c r="F103" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G103" t="s">
-        <v>157</v>
+        <v>12</v>
       </c>
       <c r="H103" t="s">
         <v>301</v>
@@ -4218,169 +4179,157 @@
         <v>302</v>
       </c>
       <c r="B104" t="s">
+        <v>248</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>283.0</v>
+      </c>
+      <c r="E104" t="s">
+        <v>10</v>
+      </c>
+      <c r="F104" t="s">
+        <v>11</v>
+      </c>
+      <c r="G104" t="s">
+        <v>20</v>
+      </c>
+      <c r="H104" t="s">
         <v>303</v>
-      </c>
-      <c r="C104">
-        <v>1</v>
-      </c>
-      <c r="D104">
-        <v>409.0</v>
-      </c>
-      <c r="E104" t="s">
-        <v>304</v>
-      </c>
-      <c r="F104" t="s">
-        <v>11</v>
-      </c>
-      <c r="G104" t="s">
-        <v>305</v>
-      </c>
-      <c r="H104" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="105" spans="1:8">
       <c r="A105" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B105" t="s">
-        <v>259</v>
+        <v>305</v>
       </c>
       <c r="C105">
         <v>1</v>
       </c>
       <c r="D105">
-        <v>303.0</v>
-      </c>
-      <c r="E105" t="s">
-        <v>10</v>
-      </c>
-      <c r="F105" t="s">
-        <v>11</v>
-      </c>
-      <c r="G105" t="s">
-        <v>20</v>
-      </c>
-      <c r="H105" t="s">
-        <v>308</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B106" t="s">
-        <v>80</v>
+        <v>164</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
       <c r="D106">
-        <v>416.0</v>
+        <v>239.0</v>
       </c>
       <c r="E106" t="s">
-        <v>58</v>
+        <v>165</v>
       </c>
       <c r="F106" t="s">
         <v>37</v>
       </c>
       <c r="G106" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H106" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B107" t="s">
-        <v>177</v>
+        <v>308</v>
       </c>
       <c r="C107">
         <v>1</v>
       </c>
       <c r="D107">
-        <v>239.0</v>
+        <v>536.0</v>
       </c>
       <c r="E107" t="s">
-        <v>178</v>
+        <v>30</v>
       </c>
       <c r="F107" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G107" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="H107" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="108" spans="1:8">
       <c r="A108" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B108" t="s">
-        <v>259</v>
+        <v>311</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
       <c r="D108">
-        <v>283.0</v>
-      </c>
-      <c r="E108" t="s">
-        <v>10</v>
-      </c>
-      <c r="F108" t="s">
-        <v>11</v>
-      </c>
-      <c r="G108" t="s">
-        <v>20</v>
-      </c>
-      <c r="H108" t="s">
-        <v>314</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="109" spans="1:8">
       <c r="A109" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B109" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C109">
         <v>1</v>
       </c>
       <c r="D109">
-        <v>1.0</v>
+        <v>179.0</v>
+      </c>
+      <c r="E109" t="s">
+        <v>10</v>
+      </c>
+      <c r="F109" t="s">
+        <v>31</v>
+      </c>
+      <c r="G109" t="s">
+        <v>12</v>
+      </c>
+      <c r="H109" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="110" spans="1:8">
       <c r="A110" t="s">
+        <v>315</v>
+      </c>
+      <c r="B110" t="s">
+        <v>29</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110">
+        <v>650.0</v>
+      </c>
+      <c r="E110" t="s">
+        <v>316</v>
+      </c>
+      <c r="F110" t="s">
+        <v>31</v>
+      </c>
+      <c r="G110" t="s">
+        <v>32</v>
+      </c>
+      <c r="H110" t="s">
         <v>317</v>
-      </c>
-      <c r="B110" t="s">
-        <v>177</v>
-      </c>
-      <c r="C110">
-        <v>1</v>
-      </c>
-      <c r="D110">
-        <v>239.0</v>
-      </c>
-      <c r="E110" t="s">
-        <v>178</v>
-      </c>
-      <c r="F110" t="s">
-        <v>37</v>
-      </c>
-      <c r="G110" t="s">
-        <v>12</v>
-      </c>
-      <c r="H110" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -4388,16 +4337,16 @@
         <v>318</v>
       </c>
       <c r="B111" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="C111">
         <v>1</v>
       </c>
       <c r="D111">
-        <v>319.0</v>
+        <v>239.0</v>
       </c>
       <c r="E111" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="F111" t="s">
         <v>11</v>
@@ -4420,16 +4369,16 @@
         <v>1</v>
       </c>
       <c r="D112">
-        <v>536.0</v>
+        <v>304.0</v>
       </c>
       <c r="E112" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F112" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G112" t="s">
-        <v>157</v>
+        <v>20</v>
       </c>
       <c r="H112" t="s">
         <v>322</v>
@@ -4446,64 +4395,76 @@
         <v>1</v>
       </c>
       <c r="D113">
-        <v>2.0</v>
+        <v>381.0</v>
+      </c>
+      <c r="E113" t="s">
+        <v>325</v>
+      </c>
+      <c r="F113" t="s">
+        <v>37</v>
+      </c>
+      <c r="G113" t="s">
+        <v>12</v>
+      </c>
+      <c r="H113" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="114" spans="1:8">
       <c r="A114" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B114" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="C114">
         <v>1</v>
       </c>
       <c r="D114">
-        <v>179.0</v>
+        <v>575.0</v>
       </c>
       <c r="E114" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F114" t="s">
         <v>31</v>
       </c>
       <c r="G114" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="H114" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="115" spans="1:8">
       <c r="A115" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B115" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C115">
         <v>1</v>
       </c>
       <c r="D115">
-        <v>650.0</v>
+        <v>50.0</v>
       </c>
       <c r="E115" t="s">
-        <v>329</v>
+        <v>41</v>
       </c>
       <c r="F115" t="s">
         <v>31</v>
       </c>
       <c r="G115" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="H115" t="s">
-        <v>330</v>
+        <v>43</v>
       </c>
     </row>
     <row r="116" spans="1:8">
       <c r="A116" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B116" t="s">
         <v>9</v>
@@ -4512,7 +4473,7 @@
         <v>1</v>
       </c>
       <c r="D116">
-        <v>239.0</v>
+        <v>219.0</v>
       </c>
       <c r="E116" t="s">
         <v>10</v>
@@ -4521,608 +4482,478 @@
         <v>11</v>
       </c>
       <c r="G116" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H116" t="s">
-        <v>332</v>
+        <v>259</v>
       </c>
     </row>
     <row r="117" spans="1:8">
       <c r="A117" t="s">
+        <v>331</v>
+      </c>
+      <c r="B117" t="s">
+        <v>332</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117">
+        <v>110.0</v>
+      </c>
+      <c r="E117" t="s">
+        <v>119</v>
+      </c>
+      <c r="F117" t="s">
+        <v>31</v>
+      </c>
+      <c r="G117" t="s">
+        <v>12</v>
+      </c>
+      <c r="H117" t="s">
         <v>333</v>
-      </c>
-      <c r="B117" t="s">
-        <v>334</v>
-      </c>
-      <c r="C117">
-        <v>1</v>
-      </c>
-      <c r="D117">
-        <v>304.0</v>
-      </c>
-      <c r="E117" t="s">
-        <v>10</v>
-      </c>
-      <c r="F117" t="s">
-        <v>11</v>
-      </c>
-      <c r="G117" t="s">
-        <v>20</v>
-      </c>
-      <c r="H117" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="118" spans="1:8">
       <c r="A118" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B118" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C118">
         <v>1</v>
       </c>
       <c r="D118">
-        <v>381.0</v>
+        <v>160.0</v>
       </c>
       <c r="E118" t="s">
-        <v>338</v>
+        <v>24</v>
       </c>
       <c r="F118" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G118" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H118" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="119" spans="1:8">
       <c r="A119" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B119" t="s">
-        <v>321</v>
+        <v>15</v>
       </c>
       <c r="C119">
         <v>1</v>
       </c>
       <c r="D119">
-        <v>575.0</v>
+        <v>208.0</v>
       </c>
       <c r="E119" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F119" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G119" t="s">
-        <v>157</v>
+        <v>20</v>
       </c>
       <c r="H119" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="120" spans="1:8">
       <c r="A120" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B120" t="s">
-        <v>40</v>
+        <v>208</v>
       </c>
       <c r="C120">
         <v>1</v>
       </c>
       <c r="D120">
-        <v>50.0</v>
+        <v>348.0</v>
       </c>
       <c r="E120" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F120" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G120" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="H120" t="s">
-        <v>43</v>
+        <v>339</v>
       </c>
     </row>
     <row r="121" spans="1:8">
       <c r="A121" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B121" t="s">
-        <v>9</v>
+        <v>308</v>
       </c>
       <c r="C121">
         <v>1</v>
       </c>
       <c r="D121">
-        <v>219.0</v>
+        <v>726.0</v>
       </c>
       <c r="E121" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F121" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G121" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="H121" t="s">
-        <v>270</v>
+        <v>341</v>
       </c>
     </row>
     <row r="122" spans="1:8">
       <c r="A122" t="s">
+        <v>342</v>
+      </c>
+      <c r="B122" t="s">
+        <v>343</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+      <c r="D122">
+        <v>428.0</v>
+      </c>
+      <c r="E122" t="s">
         <v>344</v>
       </c>
-      <c r="B122" t="s">
-        <v>345</v>
-      </c>
-      <c r="C122">
-        <v>1</v>
-      </c>
-      <c r="D122">
-        <v>110.0</v>
-      </c>
-      <c r="E122" t="s">
-        <v>127</v>
-      </c>
       <c r="F122" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G122" t="s">
         <v>12</v>
       </c>
       <c r="H122" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="123" spans="1:8">
       <c r="A123" t="s">
+        <v>346</v>
+      </c>
+      <c r="B123" t="s">
         <v>347</v>
       </c>
-      <c r="B123" t="s">
-        <v>345</v>
-      </c>
       <c r="C123">
         <v>1</v>
       </c>
       <c r="D123">
-        <v>160.0</v>
+        <v>128.0</v>
       </c>
       <c r="E123" t="s">
-        <v>24</v>
+        <v>348</v>
       </c>
       <c r="F123" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G123" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H123" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="124" spans="1:8">
       <c r="A124" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B124" t="s">
-        <v>15</v>
+        <v>351</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
       <c r="D124">
-        <v>208.0</v>
+        <v>959.0</v>
       </c>
       <c r="E124" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="F124" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G124" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="H124" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="125" spans="1:8">
       <c r="A125" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B125" t="s">
-        <v>219</v>
+        <v>155</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125">
-        <v>348.0</v>
+        <v>445.0</v>
       </c>
       <c r="E125" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F125" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G125" t="s">
         <v>32</v>
       </c>
       <c r="H125" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="126" spans="1:8">
       <c r="A126" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B126" t="s">
-        <v>321</v>
+        <v>356</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126">
-        <v>726.0</v>
+        <v>630.0</v>
       </c>
       <c r="E126" t="s">
-        <v>30</v>
+        <v>357</v>
       </c>
       <c r="F126" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G126" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="H126" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="127" spans="1:8">
       <c r="A127" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B127" t="s">
-        <v>356</v>
+        <v>243</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127">
-        <v>428.0</v>
+        <v>427.0</v>
       </c>
       <c r="E127" t="s">
-        <v>357</v>
+        <v>62</v>
       </c>
       <c r="F127" t="s">
         <v>11</v>
       </c>
       <c r="G127" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H127" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="128" spans="1:8">
       <c r="A128" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B128" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128">
-        <v>128.0</v>
+        <v>892.0</v>
       </c>
       <c r="E128" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="F128" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G128" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="H128" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="129" spans="1:8">
       <c r="A129" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B129" t="s">
-        <v>364</v>
+        <v>69</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129">
-        <v>959.0</v>
+        <v>881.0</v>
       </c>
       <c r="E129" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="F129" t="s">
         <v>31</v>
       </c>
       <c r="G129" t="s">
-        <v>157</v>
+        <v>20</v>
       </c>
       <c r="H129" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="130" spans="1:8">
       <c r="A130" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B130" t="s">
-        <v>168</v>
+        <v>368</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130">
-        <v>445.0</v>
+        <v>199.0</v>
       </c>
       <c r="E130" t="s">
-        <v>66</v>
+        <v>369</v>
       </c>
       <c r="F130" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="G130" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H130" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="131" spans="1:8">
       <c r="A131" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B131" t="s">
-        <v>369</v>
+        <v>72</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131">
-        <v>630.0</v>
+        <v>356.0</v>
       </c>
       <c r="E131" t="s">
-        <v>370</v>
+        <v>82</v>
       </c>
       <c r="F131" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G131" t="s">
-        <v>157</v>
+        <v>12</v>
       </c>
       <c r="H131" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="132" spans="1:8">
       <c r="A132" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B132" t="s">
-        <v>254</v>
+        <v>85</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132">
-        <v>427.0</v>
+        <v>376.0</v>
       </c>
       <c r="E132" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="F132" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G132" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H132" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="133" spans="1:8">
       <c r="A133" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B133" t="s">
-        <v>375</v>
+        <v>72</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133">
-        <v>892.0</v>
+        <v>396.0</v>
       </c>
       <c r="E133" t="s">
-        <v>376</v>
+        <v>82</v>
       </c>
       <c r="F133" t="s">
         <v>31</v>
       </c>
       <c r="G133" t="s">
-        <v>157</v>
+        <v>20</v>
       </c>
       <c r="H133" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="134" spans="1:8">
       <c r="A134" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B134" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134">
-        <v>881.0</v>
+        <v>475.0</v>
       </c>
       <c r="E134" t="s">
-        <v>66</v>
+        <v>363</v>
       </c>
       <c r="F134" t="s">
         <v>31</v>
       </c>
       <c r="G134" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="H134" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8">
-      <c r="A135" t="s">
-        <v>380</v>
-      </c>
-      <c r="B135" t="s">
-        <v>381</v>
-      </c>
-      <c r="C135">
-        <v>1</v>
-      </c>
-      <c r="D135">
-        <v>199.0</v>
-      </c>
-      <c r="E135" t="s">
-        <v>382</v>
-      </c>
-      <c r="F135" t="s">
-        <v>11</v>
-      </c>
-      <c r="G135" t="s">
-        <v>12</v>
-      </c>
-      <c r="H135" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8">
-      <c r="A136" t="s">
-        <v>384</v>
-      </c>
-      <c r="B136" t="s">
-        <v>76</v>
-      </c>
-      <c r="C136">
-        <v>1</v>
-      </c>
-      <c r="D136">
-        <v>356.0</v>
-      </c>
-      <c r="E136" t="s">
-        <v>90</v>
-      </c>
-      <c r="F136" t="s">
-        <v>31</v>
-      </c>
-      <c r="G136" t="s">
-        <v>12</v>
-      </c>
-      <c r="H136" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8">
-      <c r="A137" t="s">
-        <v>386</v>
-      </c>
-      <c r="B137" t="s">
-        <v>93</v>
-      </c>
-      <c r="C137">
-        <v>1</v>
-      </c>
-      <c r="D137">
-        <v>376.0</v>
-      </c>
-      <c r="E137" t="s">
-        <v>58</v>
-      </c>
-      <c r="F137" t="s">
-        <v>31</v>
-      </c>
-      <c r="G137" t="s">
-        <v>12</v>
-      </c>
-      <c r="H137" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8">
-      <c r="A138" t="s">
-        <v>388</v>
-      </c>
-      <c r="B138" t="s">
-        <v>76</v>
-      </c>
-      <c r="C138">
-        <v>1</v>
-      </c>
-      <c r="D138">
-        <v>396.0</v>
-      </c>
-      <c r="E138" t="s">
-        <v>90</v>
-      </c>
-      <c r="F138" t="s">
-        <v>31</v>
-      </c>
-      <c r="G138" t="s">
-        <v>20</v>
-      </c>
-      <c r="H138" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8">
-      <c r="A139" t="s">
-        <v>390</v>
-      </c>
-      <c r="B139" t="s">
-        <v>197</v>
-      </c>
-      <c r="C139">
-        <v>1</v>
-      </c>
-      <c r="D139">
-        <v>475.0</v>
-      </c>
-      <c r="E139" t="s">
-        <v>376</v>
-      </c>
-      <c r="F139" t="s">
-        <v>31</v>
-      </c>
-      <c r="G139" t="s">
-        <v>157</v>
-      </c>
-      <c r="H139" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -5260,11 +5091,6 @@
     <hyperlink ref="A132" r:id="rId_hyperlink_131"/>
     <hyperlink ref="A133" r:id="rId_hyperlink_132"/>
     <hyperlink ref="A134" r:id="rId_hyperlink_133"/>
-    <hyperlink ref="A135" r:id="rId_hyperlink_134"/>
-    <hyperlink ref="A136" r:id="rId_hyperlink_135"/>
-    <hyperlink ref="A137" r:id="rId_hyperlink_136"/>
-    <hyperlink ref="A138" r:id="rId_hyperlink_137"/>
-    <hyperlink ref="A139" r:id="rId_hyperlink_138"/>
   </hyperlinks>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Google Drive OAuth logic to use .env for CREDENTIALS_JSON and TOKEN_JSON
</commit_message>
<xml_diff>
--- a/DFS_LIST.XLSX
+++ b/DFS_LIST.XLSX
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="363">
   <si>
     <t>Product ID</t>
   </si>
@@ -494,12 +494,6 @@
     <t>LAT 5420 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i7Q (i7-1185G7) 3.00GHz 32GB 512GB NoOPT 32MB BkLIT W10P64</t>
   </si>
   <si>
-    <t>dell-latitude-5410-000457</t>
-  </si>
-  <si>
-    <t>LAT 5410 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-10310U) 1.70GHz 16GB 256GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
     <t>dell-latitude-5420-000440</t>
   </si>
   <si>
@@ -647,12 +641,6 @@
     <t>LAT 5520 NB STD 15.6-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-1145G7) 2.60GHz 16GB 256GB NoOPT 32MB BkLIT W10P64</t>
   </si>
   <si>
-    <t>dell-latitude-5410-000486</t>
-  </si>
-  <si>
-    <t>LAT 5410 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-10210U) 1.60GHz 16GB 256GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
     <t>dell-latitude-7420-000260</t>
   </si>
   <si>
@@ -713,21 +701,6 @@
     <t>LAT 5320 NB STD 13.3-in (1920 x 1080) TCH CAM 1x i5Q (i5-1145G7) 2.60GHz 16GB 512GB NoOPT 32MB BkLIT W10P64</t>
   </si>
   <si>
-    <t>dell-latitude-5410-000493</t>
-  </si>
-  <si>
-    <t>LAT 5410 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-10310U) 1.70GHz 8GB 256GB NoOPT 32MB NoBkLIT W10P64</t>
-  </si>
-  <si>
-    <t>dell-precision-5760-000028</t>
-  </si>
-  <si>
-    <t>Dell Precision 5760</t>
-  </si>
-  <si>
-    <t>PRE 5760 NB STD 17-in (1920 x 1200) NoTCH CAM 1x i78C (i7-11850H) 2.50GHz 16GB 256GB NoOPT 4GB BkLIT W10P64</t>
-  </si>
-  <si>
     <t>dell-latitude-3410-000025</t>
   </si>
   <si>
@@ -845,12 +818,6 @@
     <t>LAT 5520 NB STD 15.6-in (1920 x 1080) NoTCH CAM 1x i7Q (i7-1185G7) 3.00GHz 16GB 512GB NoOPT 32MB BkLIT W10P64</t>
   </si>
   <si>
-    <t>dell-latitude-5410-000498</t>
-  </si>
-  <si>
-    <t>LAT 5410 NB STD 14-in (1366 x 768) NoTCH CAM 1x i5Q (i5-10310U) 1.70GHz 8GB 256GB NoOPT 32MB BkLIT W10P64</t>
-  </si>
-  <si>
     <t>dell-latitude-7420-touch-000121</t>
   </si>
   <si>
@@ -953,15 +920,6 @@
     <t>chargeTestFinale</t>
   </si>
   <si>
-    <t>dell-latitude-5410-no-os-000065</t>
-  </si>
-  <si>
-    <t>Dell Latitude 5410 - No OS</t>
-  </si>
-  <si>
-    <t>LAT 5410 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-10310U) 1.70GHz 8GB 256GB NoOPT 32MB BkLIT NoOS</t>
-  </si>
-  <si>
     <t>microsoft-surface-laptop-3-touch-no-os-000026</t>
   </si>
   <si>
@@ -969,12 +927,6 @@
   </si>
   <si>
     <t>SUR Laptop 3 NB STD 13.5-in (2256 x 1504) TCH CAM 1x i5 (i5-1035G7) 1.20GHz 16GB 256GB NoOPT 32MB BkLIT NoOS</t>
-  </si>
-  <si>
-    <t>dell-latitude-5410-000505</t>
-  </si>
-  <si>
-    <t>LAT 5410 NB STD 14-in (1920 x 1080) NoTCH CAM 1x i5Q (i5-10310U) 1.70GHz 16GB 256GB NoOPT 32MB NoBkLIT W10P64</t>
   </si>
   <si>
     <t>dell-latitude-7410-000212</t>
@@ -1491,7 +1443,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H134"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -2775,22 +2727,22 @@
         <v>159</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <v>249.0</v>
+        <v>335.0</v>
       </c>
       <c r="E50" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="F50" t="s">
         <v>11</v>
       </c>
       <c r="G50" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H50" t="s">
         <v>160</v>
@@ -2801,48 +2753,48 @@
         <v>161</v>
       </c>
       <c r="B51" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>335.0</v>
+        <v>230.0</v>
       </c>
       <c r="E51" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
       <c r="F51" t="s">
         <v>11</v>
       </c>
       <c r="G51" t="s">
-        <v>20</v>
+        <v>164</v>
       </c>
       <c r="H51" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B52" t="s">
-        <v>164</v>
+        <v>35</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52">
-        <v>230.0</v>
+        <v>386.0</v>
       </c>
       <c r="E52" t="s">
-        <v>165</v>
+        <v>54</v>
       </c>
       <c r="F52" t="s">
         <v>11</v>
       </c>
       <c r="G52" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="H52" t="s">
         <v>167</v>
@@ -2853,16 +2805,16 @@
         <v>168</v>
       </c>
       <c r="B53" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53">
-        <v>386.0</v>
+        <v>218.0</v>
       </c>
       <c r="E53" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="F53" t="s">
         <v>11</v>
@@ -2885,7 +2837,7 @@
         <v>1</v>
       </c>
       <c r="D54">
-        <v>218.0</v>
+        <v>209.0</v>
       </c>
       <c r="E54" t="s">
         <v>16</v>
@@ -2894,15 +2846,15 @@
         <v>11</v>
       </c>
       <c r="G54" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="H54" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
@@ -2911,7 +2863,7 @@
         <v>1</v>
       </c>
       <c r="D55">
-        <v>209.0</v>
+        <v>199.0</v>
       </c>
       <c r="E55" t="s">
         <v>16</v>
@@ -2920,27 +2872,27 @@
         <v>11</v>
       </c>
       <c r="G55" t="s">
-        <v>173</v>
+        <v>12</v>
       </c>
       <c r="H55" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
+        <v>174</v>
+      </c>
+      <c r="B56" t="s">
         <v>175</v>
       </c>
-      <c r="B56" t="s">
-        <v>15</v>
-      </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56">
-        <v>199.0</v>
+        <v>288.0</v>
       </c>
       <c r="E56" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="F56" t="s">
         <v>11</v>
@@ -2949,30 +2901,30 @@
         <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B57" t="s">
-        <v>177</v>
+        <v>15</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57">
-        <v>288.0</v>
+        <v>219.0</v>
       </c>
       <c r="E57" t="s">
-        <v>178</v>
+        <v>16</v>
       </c>
       <c r="F57" t="s">
         <v>11</v>
       </c>
       <c r="G57" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H57" t="s">
         <v>179</v>
@@ -2998,7 +2950,7 @@
         <v>11</v>
       </c>
       <c r="G58" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H58" t="s">
         <v>181</v>
@@ -3009,152 +2961,152 @@
         <v>182</v>
       </c>
       <c r="B59" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59">
-        <v>219.0</v>
+        <v>352.0</v>
       </c>
       <c r="E59" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F59" t="s">
         <v>11</v>
       </c>
       <c r="G59" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="H59" t="s">
-        <v>183</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
+        <v>183</v>
+      </c>
+      <c r="B60" t="s">
         <v>184</v>
       </c>
-      <c r="B60" t="s">
-        <v>19</v>
-      </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60">
-        <v>352.0</v>
+        <v>475.0</v>
       </c>
       <c r="E60" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="F60" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G60" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="H60" t="s">
-        <v>145</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B61" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61">
-        <v>475.0</v>
+        <v>425.0</v>
       </c>
       <c r="E61" t="s">
-        <v>101</v>
+        <v>147</v>
       </c>
       <c r="F61" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G61" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="H61" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B62" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62">
-        <v>425.0</v>
+        <v>401.0</v>
       </c>
       <c r="E62" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
       <c r="F62" t="s">
         <v>11</v>
       </c>
       <c r="G62" t="s">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="H62" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B63" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63">
-        <v>401.0</v>
+        <v>261.0</v>
       </c>
       <c r="E63" t="s">
-        <v>193</v>
+        <v>127</v>
       </c>
       <c r="F63" t="s">
         <v>11</v>
       </c>
       <c r="G63" t="s">
-        <v>194</v>
+        <v>32</v>
       </c>
       <c r="H63" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B64" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64">
-        <v>261.0</v>
+        <v>249.0</v>
       </c>
       <c r="E64" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="F64" t="s">
         <v>11</v>
       </c>
       <c r="G64" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="H64" t="s">
         <v>198</v>
@@ -3165,22 +3117,22 @@
         <v>199</v>
       </c>
       <c r="B65" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65">
-        <v>249.0</v>
+        <v>189.0</v>
       </c>
       <c r="E65" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F65" t="s">
         <v>11</v>
       </c>
       <c r="G65" t="s">
-        <v>144</v>
+        <v>12</v>
       </c>
       <c r="H65" t="s">
         <v>200</v>
@@ -3191,42 +3143,42 @@
         <v>201</v>
       </c>
       <c r="B66" t="s">
-        <v>164</v>
+        <v>202</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66">
-        <v>189.0</v>
+        <v>253.0</v>
       </c>
       <c r="E66" t="s">
-        <v>165</v>
+        <v>203</v>
       </c>
       <c r="F66" t="s">
         <v>11</v>
       </c>
       <c r="G66" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H66" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B67" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67">
-        <v>253.0</v>
+        <v>348.0</v>
       </c>
       <c r="E67" t="s">
-        <v>205</v>
+        <v>82</v>
       </c>
       <c r="F67" t="s">
         <v>11</v>
@@ -3235,30 +3187,30 @@
         <v>32</v>
       </c>
       <c r="H67" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B68" t="s">
-        <v>208</v>
+        <v>104</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68">
-        <v>348.0</v>
+        <v>520.0</v>
       </c>
       <c r="E68" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="F68" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G68" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="H68" t="s">
         <v>209</v>
@@ -3269,100 +3221,100 @@
         <v>210</v>
       </c>
       <c r="B69" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69">
-        <v>249.0</v>
+        <v>421.0</v>
       </c>
       <c r="E69" t="s">
-        <v>97</v>
+        <v>211</v>
       </c>
       <c r="F69" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G69" t="s">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="H69" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B70" t="s">
-        <v>104</v>
+        <v>214</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70">
-        <v>520.0</v>
+        <v>619.0</v>
       </c>
       <c r="E70" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="F70" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="G70" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="H70" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B71" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71">
-        <v>421.0</v>
+        <v>328.0</v>
       </c>
       <c r="E71" t="s">
-        <v>215</v>
+        <v>82</v>
       </c>
       <c r="F71" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="G71" t="s">
-        <v>194</v>
+        <v>12</v>
       </c>
       <c r="H71" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B72" t="s">
-        <v>218</v>
+        <v>155</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72">
-        <v>619.0</v>
+        <v>395.0</v>
       </c>
       <c r="E72" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="F72" t="s">
         <v>11</v>
       </c>
       <c r="G72" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="H72" t="s">
         <v>219</v>
@@ -3373,68 +3325,68 @@
         <v>220</v>
       </c>
       <c r="B73" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73">
-        <v>328.0</v>
+        <v>419.0</v>
       </c>
       <c r="E73" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="F73" t="s">
         <v>11</v>
       </c>
       <c r="G73" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H73" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B74" t="s">
-        <v>155</v>
+        <v>224</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74">
-        <v>395.0</v>
+        <v>416.0</v>
       </c>
       <c r="E74" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="F74" t="s">
         <v>11</v>
       </c>
       <c r="G74" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H74" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B75" t="s">
-        <v>225</v>
+        <v>65</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75">
-        <v>419.0</v>
+        <v>368.0</v>
       </c>
       <c r="E75" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="F75" t="s">
         <v>11</v>
@@ -3443,128 +3395,128 @@
         <v>20</v>
       </c>
       <c r="H75" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B76" t="s">
-        <v>228</v>
+        <v>96</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76">
-        <v>416.0</v>
+        <v>211.0</v>
       </c>
       <c r="E76" t="s">
-        <v>147</v>
+        <v>229</v>
       </c>
       <c r="F76" t="s">
         <v>11</v>
       </c>
       <c r="G76" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H76" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B77" t="s">
-        <v>65</v>
+        <v>214</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77">
-        <v>368.0</v>
+        <v>520.0</v>
       </c>
       <c r="E77" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="F77" t="s">
         <v>11</v>
       </c>
       <c r="G77" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H77" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B78" t="s">
-        <v>9</v>
+        <v>234</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78">
-        <v>219.0</v>
+        <v>418.0</v>
       </c>
       <c r="E78" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="F78" t="s">
         <v>11</v>
       </c>
       <c r="G78" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="H78" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B79" t="s">
-        <v>235</v>
+        <v>81</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79">
-        <v>566.0</v>
+        <v>530.0</v>
       </c>
       <c r="E79" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="F79" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G79" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H79" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B80" t="s">
-        <v>96</v>
+        <v>239</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80">
-        <v>211.0</v>
+        <v>248.0</v>
       </c>
       <c r="E80" t="s">
-        <v>238</v>
+        <v>10</v>
       </c>
       <c r="F80" t="s">
         <v>11</v>
@@ -3573,99 +3525,99 @@
         <v>12</v>
       </c>
       <c r="H80" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B81" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81">
-        <v>520.0</v>
+        <v>328.0</v>
       </c>
       <c r="E81" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="F81" t="s">
         <v>11</v>
       </c>
       <c r="G81" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H81" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B82" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82">
-        <v>418.0</v>
+        <v>120.0</v>
       </c>
       <c r="E82" t="s">
-        <v>62</v>
+        <v>245</v>
       </c>
       <c r="F82" t="s">
         <v>11</v>
       </c>
       <c r="G82" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="H82" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B83" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
       <c r="D83">
-        <v>530.0</v>
+        <v>811.0</v>
       </c>
       <c r="E83" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="F83" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G83" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H83" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B84" t="s">
-        <v>248</v>
+        <v>9</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
       <c r="D84">
-        <v>248.0</v>
+        <v>219.0</v>
       </c>
       <c r="E84" t="s">
         <v>10</v>
@@ -3674,59 +3626,59 @@
         <v>11</v>
       </c>
       <c r="G84" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H84" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B85" t="s">
-        <v>208</v>
+        <v>72</v>
       </c>
       <c r="C85">
         <v>1</v>
       </c>
       <c r="D85">
-        <v>328.0</v>
+        <v>436.0</v>
       </c>
       <c r="E85" t="s">
-        <v>54</v>
+        <v>147</v>
       </c>
       <c r="F85" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G85" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="H85" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B86" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
       <c r="D86">
-        <v>120.0</v>
+        <v>336.0</v>
       </c>
       <c r="E86" t="s">
-        <v>254</v>
+        <v>147</v>
       </c>
       <c r="F86" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G86" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="H86" t="s">
         <v>255</v>
@@ -3737,126 +3689,126 @@
         <v>256</v>
       </c>
       <c r="B87" t="s">
-        <v>69</v>
+        <v>257</v>
       </c>
       <c r="C87">
         <v>1</v>
       </c>
       <c r="D87">
-        <v>811.0</v>
+        <v>525.0</v>
       </c>
       <c r="E87" t="s">
-        <v>82</v>
+        <v>258</v>
       </c>
       <c r="F87" t="s">
         <v>31</v>
       </c>
       <c r="G87" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="H87" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>261</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
       <c r="D88">
-        <v>219.0</v>
+        <v>691.0</v>
       </c>
       <c r="E88" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="F88" t="s">
         <v>11</v>
       </c>
       <c r="G88" t="s">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="H88" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B89" t="s">
-        <v>72</v>
+        <v>221</v>
       </c>
       <c r="C89">
         <v>1</v>
       </c>
       <c r="D89">
-        <v>436.0</v>
+        <v>314.0</v>
       </c>
       <c r="E89" t="s">
-        <v>147</v>
+        <v>10</v>
       </c>
       <c r="F89" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G89" t="s">
-        <v>144</v>
+        <v>12</v>
       </c>
       <c r="H89" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B90" t="s">
-        <v>263</v>
+        <v>206</v>
       </c>
       <c r="C90">
         <v>1</v>
       </c>
       <c r="D90">
-        <v>336.0</v>
+        <v>418.0</v>
       </c>
       <c r="E90" t="s">
-        <v>147</v>
+        <v>62</v>
       </c>
       <c r="F90" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G90" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H90" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="91" spans="1:8">
       <c r="A91" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B91" t="s">
-        <v>266</v>
+        <v>81</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
       <c r="D91">
-        <v>525.0</v>
+        <v>460.0</v>
       </c>
       <c r="E91" t="s">
-        <v>267</v>
+        <v>62</v>
       </c>
       <c r="F91" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G91" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="H91" t="s">
         <v>268</v>
@@ -3867,22 +3819,22 @@
         <v>269</v>
       </c>
       <c r="B92" t="s">
+        <v>96</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>301.0</v>
+      </c>
+      <c r="E92" t="s">
+        <v>97</v>
+      </c>
+      <c r="F92" t="s">
         <v>270</v>
       </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-      <c r="D92">
-        <v>691.0</v>
-      </c>
-      <c r="E92" t="s">
-        <v>86</v>
-      </c>
-      <c r="F92" t="s">
-        <v>11</v>
-      </c>
       <c r="G92" t="s">
-        <v>194</v>
+        <v>12</v>
       </c>
       <c r="H92" t="s">
         <v>271</v>
@@ -3893,94 +3845,94 @@
         <v>272</v>
       </c>
       <c r="B93" t="s">
-        <v>225</v>
+        <v>273</v>
       </c>
       <c r="C93">
         <v>1</v>
       </c>
       <c r="D93">
-        <v>314.0</v>
+        <v>455.0</v>
       </c>
       <c r="E93" t="s">
-        <v>10</v>
+        <v>274</v>
       </c>
       <c r="F93" t="s">
         <v>11</v>
       </c>
       <c r="G93" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H93" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="94" spans="1:8">
       <c r="A94" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B94" t="s">
-        <v>208</v>
+        <v>277</v>
       </c>
       <c r="C94">
         <v>1</v>
       </c>
       <c r="D94">
-        <v>418.0</v>
+        <v>1134.0</v>
       </c>
       <c r="E94" t="s">
-        <v>62</v>
+        <v>278</v>
       </c>
       <c r="F94" t="s">
         <v>11</v>
       </c>
       <c r="G94" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="H94" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B95" t="s">
-        <v>9</v>
+        <v>281</v>
       </c>
       <c r="C95">
         <v>1</v>
       </c>
       <c r="D95">
-        <v>214.0</v>
+        <v>409.0</v>
       </c>
       <c r="E95" t="s">
-        <v>10</v>
+        <v>282</v>
       </c>
       <c r="F95" t="s">
         <v>11</v>
       </c>
       <c r="G95" t="s">
-        <v>12</v>
+        <v>283</v>
       </c>
       <c r="H95" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="B96" t="s">
-        <v>81</v>
+        <v>239</v>
       </c>
       <c r="C96">
         <v>1</v>
       </c>
       <c r="D96">
-        <v>460.0</v>
+        <v>303.0</v>
       </c>
       <c r="E96" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="F96" t="s">
         <v>11</v>
@@ -3989,212 +3941,188 @@
         <v>20</v>
       </c>
       <c r="H96" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="B97" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="C97">
         <v>1</v>
       </c>
       <c r="D97">
-        <v>301.0</v>
+        <v>416.0</v>
       </c>
       <c r="E97" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="F97" t="s">
-        <v>281</v>
+        <v>37</v>
       </c>
       <c r="G97" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H97" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="B98" t="s">
-        <v>284</v>
+        <v>162</v>
       </c>
       <c r="C98">
         <v>1</v>
       </c>
       <c r="D98">
-        <v>455.0</v>
+        <v>239.0</v>
       </c>
       <c r="E98" t="s">
-        <v>285</v>
+        <v>163</v>
       </c>
       <c r="F98" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G98" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H98" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B99" t="s">
-        <v>288</v>
+        <v>239</v>
       </c>
       <c r="C99">
         <v>1</v>
       </c>
       <c r="D99">
-        <v>1134.0</v>
+        <v>283.0</v>
       </c>
       <c r="E99" t="s">
-        <v>289</v>
+        <v>10</v>
       </c>
       <c r="F99" t="s">
         <v>11</v>
       </c>
       <c r="G99" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="H99" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B100" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C100">
         <v>1</v>
       </c>
       <c r="D100">
-        <v>409.0</v>
-      </c>
-      <c r="E100" t="s">
-        <v>293</v>
-      </c>
-      <c r="F100" t="s">
-        <v>11</v>
-      </c>
-      <c r="G100" t="s">
-        <v>294</v>
-      </c>
-      <c r="H100" t="s">
-        <v>295</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="101" spans="1:8">
       <c r="A101" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B101" t="s">
-        <v>248</v>
+        <v>162</v>
       </c>
       <c r="C101">
         <v>1</v>
       </c>
       <c r="D101">
-        <v>303.0</v>
+        <v>239.0</v>
       </c>
       <c r="E101" t="s">
-        <v>10</v>
+        <v>163</v>
       </c>
       <c r="F101" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G101" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H101" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
+        <v>296</v>
+      </c>
+      <c r="B102" t="s">
+        <v>297</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>536.0</v>
+      </c>
+      <c r="E102" t="s">
+        <v>30</v>
+      </c>
+      <c r="F102" t="s">
+        <v>31</v>
+      </c>
+      <c r="G102" t="s">
+        <v>144</v>
+      </c>
+      <c r="H102" t="s">
         <v>298</v>
-      </c>
-      <c r="B102" t="s">
-        <v>76</v>
-      </c>
-      <c r="C102">
-        <v>1</v>
-      </c>
-      <c r="D102">
-        <v>416.0</v>
-      </c>
-      <c r="E102" t="s">
-        <v>54</v>
-      </c>
-      <c r="F102" t="s">
-        <v>37</v>
-      </c>
-      <c r="G102" t="s">
-        <v>20</v>
-      </c>
-      <c r="H102" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
+        <v>299</v>
+      </c>
+      <c r="B103" t="s">
         <v>300</v>
       </c>
-      <c r="B103" t="s">
-        <v>164</v>
-      </c>
       <c r="C103">
         <v>1</v>
       </c>
       <c r="D103">
-        <v>239.0</v>
-      </c>
-      <c r="E103" t="s">
-        <v>165</v>
-      </c>
-      <c r="F103" t="s">
-        <v>37</v>
-      </c>
-      <c r="G103" t="s">
-        <v>12</v>
-      </c>
-      <c r="H103" t="s">
-        <v>301</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="104" spans="1:8">
       <c r="A104" t="s">
+        <v>301</v>
+      </c>
+      <c r="B104" t="s">
+        <v>29</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>650.0</v>
+      </c>
+      <c r="E104" t="s">
         <v>302</v>
       </c>
-      <c r="B104" t="s">
-        <v>248</v>
-      </c>
-      <c r="C104">
-        <v>1</v>
-      </c>
-      <c r="D104">
-        <v>283.0</v>
-      </c>
-      <c r="E104" t="s">
-        <v>10</v>
-      </c>
       <c r="F104" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G104" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H104" t="s">
         <v>303</v>
@@ -4211,24 +4139,36 @@
         <v>1</v>
       </c>
       <c r="D105">
-        <v>1.0</v>
+        <v>304.0</v>
+      </c>
+      <c r="E105" t="s">
+        <v>10</v>
+      </c>
+      <c r="F105" t="s">
+        <v>11</v>
+      </c>
+      <c r="G105" t="s">
+        <v>20</v>
+      </c>
+      <c r="H105" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B106" t="s">
-        <v>164</v>
+        <v>308</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
       <c r="D106">
-        <v>239.0</v>
+        <v>381.0</v>
       </c>
       <c r="E106" t="s">
-        <v>165</v>
+        <v>309</v>
       </c>
       <c r="F106" t="s">
         <v>37</v>
@@ -4237,21 +4177,21 @@
         <v>12</v>
       </c>
       <c r="H106" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B107" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="C107">
         <v>1</v>
       </c>
       <c r="D107">
-        <v>536.0</v>
+        <v>575.0</v>
       </c>
       <c r="E107" t="s">
         <v>30</v>
@@ -4263,47 +4203,59 @@
         <v>144</v>
       </c>
       <c r="H107" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="108" spans="1:8">
       <c r="A108" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B108" t="s">
-        <v>311</v>
+        <v>40</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
       <c r="D108">
-        <v>2.0</v>
+        <v>50.0</v>
+      </c>
+      <c r="E108" t="s">
+        <v>41</v>
+      </c>
+      <c r="F108" t="s">
+        <v>31</v>
+      </c>
+      <c r="G108" t="s">
+        <v>42</v>
+      </c>
+      <c r="H108" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="109" spans="1:8">
       <c r="A109" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B109" t="s">
-        <v>313</v>
+        <v>9</v>
       </c>
       <c r="C109">
         <v>1</v>
       </c>
       <c r="D109">
-        <v>179.0</v>
+        <v>219.0</v>
       </c>
       <c r="E109" t="s">
         <v>10</v>
       </c>
       <c r="F109" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="G109" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H109" t="s">
-        <v>314</v>
+        <v>250</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -4311,22 +4263,22 @@
         <v>315</v>
       </c>
       <c r="B110" t="s">
-        <v>29</v>
+        <v>316</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
       <c r="D110">
-        <v>650.0</v>
+        <v>110.0</v>
       </c>
       <c r="E110" t="s">
-        <v>316</v>
+        <v>119</v>
       </c>
       <c r="F110" t="s">
         <v>31</v>
       </c>
       <c r="G110" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H110" t="s">
         <v>317</v>
@@ -4337,19 +4289,19 @@
         <v>318</v>
       </c>
       <c r="B111" t="s">
-        <v>9</v>
+        <v>316</v>
       </c>
       <c r="C111">
         <v>1</v>
       </c>
       <c r="D111">
-        <v>239.0</v>
+        <v>160.0</v>
       </c>
       <c r="E111" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F111" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G111" t="s">
         <v>32</v>
@@ -4363,16 +4315,16 @@
         <v>320</v>
       </c>
       <c r="B112" t="s">
-        <v>321</v>
+        <v>15</v>
       </c>
       <c r="C112">
         <v>1</v>
       </c>
       <c r="D112">
-        <v>304.0</v>
+        <v>208.0</v>
       </c>
       <c r="E112" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F112" t="s">
         <v>11</v>
@@ -4381,47 +4333,47 @@
         <v>20</v>
       </c>
       <c r="H112" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="113" spans="1:8">
       <c r="A113" t="s">
+        <v>322</v>
+      </c>
+      <c r="B113" t="s">
+        <v>206</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113">
+        <v>348.0</v>
+      </c>
+      <c r="E113" t="s">
+        <v>54</v>
+      </c>
+      <c r="F113" t="s">
+        <v>11</v>
+      </c>
+      <c r="G113" t="s">
+        <v>32</v>
+      </c>
+      <c r="H113" t="s">
         <v>323</v>
-      </c>
-      <c r="B113" t="s">
-        <v>324</v>
-      </c>
-      <c r="C113">
-        <v>1</v>
-      </c>
-      <c r="D113">
-        <v>381.0</v>
-      </c>
-      <c r="E113" t="s">
-        <v>325</v>
-      </c>
-      <c r="F113" t="s">
-        <v>37</v>
-      </c>
-      <c r="G113" t="s">
-        <v>12</v>
-      </c>
-      <c r="H113" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="114" spans="1:8">
       <c r="A114" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B114" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="C114">
         <v>1</v>
       </c>
       <c r="D114">
-        <v>575.0</v>
+        <v>726.0</v>
       </c>
       <c r="E114" t="s">
         <v>30</v>
@@ -4433,33 +4385,33 @@
         <v>144</v>
       </c>
       <c r="H114" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="115" spans="1:8">
       <c r="A115" t="s">
+        <v>326</v>
+      </c>
+      <c r="B115" t="s">
+        <v>327</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115">
+        <v>428.0</v>
+      </c>
+      <c r="E115" t="s">
+        <v>328</v>
+      </c>
+      <c r="F115" t="s">
+        <v>11</v>
+      </c>
+      <c r="G115" t="s">
+        <v>12</v>
+      </c>
+      <c r="H115" t="s">
         <v>329</v>
-      </c>
-      <c r="B115" t="s">
-        <v>40</v>
-      </c>
-      <c r="C115">
-        <v>1</v>
-      </c>
-      <c r="D115">
-        <v>50.0</v>
-      </c>
-      <c r="E115" t="s">
-        <v>41</v>
-      </c>
-      <c r="F115" t="s">
-        <v>31</v>
-      </c>
-      <c r="G115" t="s">
-        <v>42</v>
-      </c>
-      <c r="H115" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4467,146 +4419,146 @@
         <v>330</v>
       </c>
       <c r="B116" t="s">
-        <v>9</v>
+        <v>331</v>
       </c>
       <c r="C116">
         <v>1</v>
       </c>
       <c r="D116">
-        <v>219.0</v>
+        <v>128.0</v>
       </c>
       <c r="E116" t="s">
-        <v>10</v>
+        <v>332</v>
       </c>
       <c r="F116" t="s">
         <v>11</v>
       </c>
       <c r="G116" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H116" t="s">
-        <v>259</v>
+        <v>333</v>
       </c>
     </row>
     <row r="117" spans="1:8">
       <c r="A117" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B117" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C117">
         <v>1</v>
       </c>
       <c r="D117">
-        <v>110.0</v>
+        <v>959.0</v>
       </c>
       <c r="E117" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="F117" t="s">
         <v>31</v>
       </c>
       <c r="G117" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="H117" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="118" spans="1:8">
       <c r="A118" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B118" t="s">
-        <v>332</v>
+        <v>155</v>
       </c>
       <c r="C118">
         <v>1</v>
       </c>
       <c r="D118">
-        <v>160.0</v>
+        <v>445.0</v>
       </c>
       <c r="E118" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="F118" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G118" t="s">
         <v>32</v>
       </c>
       <c r="H118" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="119" spans="1:8">
       <c r="A119" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B119" t="s">
-        <v>15</v>
+        <v>340</v>
       </c>
       <c r="C119">
         <v>1</v>
       </c>
       <c r="D119">
-        <v>208.0</v>
+        <v>630.0</v>
       </c>
       <c r="E119" t="s">
-        <v>16</v>
+        <v>341</v>
       </c>
       <c r="F119" t="s">
         <v>11</v>
       </c>
       <c r="G119" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="H119" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
     </row>
     <row r="120" spans="1:8">
       <c r="A120" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="B120" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="C120">
         <v>1</v>
       </c>
       <c r="D120">
-        <v>348.0</v>
+        <v>427.0</v>
       </c>
       <c r="E120" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F120" t="s">
         <v>11</v>
       </c>
       <c r="G120" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H120" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="121" spans="1:8">
       <c r="A121" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="B121" t="s">
-        <v>308</v>
+        <v>346</v>
       </c>
       <c r="C121">
         <v>1</v>
       </c>
       <c r="D121">
-        <v>726.0</v>
+        <v>892.0</v>
       </c>
       <c r="E121" t="s">
-        <v>30</v>
+        <v>347</v>
       </c>
       <c r="F121" t="s">
         <v>31</v>
@@ -4615,50 +4567,50 @@
         <v>144</v>
       </c>
       <c r="H121" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
     </row>
     <row r="122" spans="1:8">
       <c r="A122" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="B122" t="s">
-        <v>343</v>
+        <v>69</v>
       </c>
       <c r="C122">
         <v>1</v>
       </c>
       <c r="D122">
-        <v>428.0</v>
+        <v>881.0</v>
       </c>
       <c r="E122" t="s">
-        <v>344</v>
+        <v>62</v>
       </c>
       <c r="F122" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G122" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H122" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="123" spans="1:8">
       <c r="A123" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="B123" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="C123">
         <v>1</v>
       </c>
       <c r="D123">
-        <v>128.0</v>
+        <v>199.0</v>
       </c>
       <c r="E123" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="F123" t="s">
         <v>11</v>
@@ -4667,293 +4619,111 @@
         <v>12</v>
       </c>
       <c r="H123" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="124" spans="1:8">
       <c r="A124" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="B124" t="s">
-        <v>351</v>
+        <v>72</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
       <c r="D124">
-        <v>959.0</v>
+        <v>356.0</v>
       </c>
       <c r="E124" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="F124" t="s">
         <v>31</v>
       </c>
       <c r="G124" t="s">
-        <v>144</v>
+        <v>12</v>
       </c>
       <c r="H124" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="125" spans="1:8">
       <c r="A125" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B125" t="s">
-        <v>155</v>
+        <v>85</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125">
-        <v>445.0</v>
+        <v>376.0</v>
       </c>
       <c r="E125" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F125" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G125" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H125" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="126" spans="1:8">
       <c r="A126" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B126" t="s">
-        <v>356</v>
+        <v>72</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126">
-        <v>630.0</v>
+        <v>396.0</v>
       </c>
       <c r="E126" t="s">
-        <v>357</v>
+        <v>82</v>
       </c>
       <c r="F126" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G126" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="H126" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="127" spans="1:8">
       <c r="A127" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B127" t="s">
-        <v>243</v>
+        <v>184</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127">
-        <v>427.0</v>
+        <v>475.0</v>
       </c>
       <c r="E127" t="s">
-        <v>62</v>
+        <v>347</v>
       </c>
       <c r="F127" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G127" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="H127" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8">
-      <c r="A128" t="s">
-        <v>361</v>
-      </c>
-      <c r="B128" t="s">
         <v>362</v>
-      </c>
-      <c r="C128">
-        <v>1</v>
-      </c>
-      <c r="D128">
-        <v>892.0</v>
-      </c>
-      <c r="E128" t="s">
-        <v>363</v>
-      </c>
-      <c r="F128" t="s">
-        <v>31</v>
-      </c>
-      <c r="G128" t="s">
-        <v>144</v>
-      </c>
-      <c r="H128" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8">
-      <c r="A129" t="s">
-        <v>365</v>
-      </c>
-      <c r="B129" t="s">
-        <v>69</v>
-      </c>
-      <c r="C129">
-        <v>1</v>
-      </c>
-      <c r="D129">
-        <v>881.0</v>
-      </c>
-      <c r="E129" t="s">
-        <v>62</v>
-      </c>
-      <c r="F129" t="s">
-        <v>31</v>
-      </c>
-      <c r="G129" t="s">
-        <v>20</v>
-      </c>
-      <c r="H129" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8">
-      <c r="A130" t="s">
-        <v>367</v>
-      </c>
-      <c r="B130" t="s">
-        <v>368</v>
-      </c>
-      <c r="C130">
-        <v>1</v>
-      </c>
-      <c r="D130">
-        <v>199.0</v>
-      </c>
-      <c r="E130" t="s">
-        <v>369</v>
-      </c>
-      <c r="F130" t="s">
-        <v>11</v>
-      </c>
-      <c r="G130" t="s">
-        <v>12</v>
-      </c>
-      <c r="H130" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8">
-      <c r="A131" t="s">
-        <v>371</v>
-      </c>
-      <c r="B131" t="s">
-        <v>72</v>
-      </c>
-      <c r="C131">
-        <v>1</v>
-      </c>
-      <c r="D131">
-        <v>356.0</v>
-      </c>
-      <c r="E131" t="s">
-        <v>82</v>
-      </c>
-      <c r="F131" t="s">
-        <v>31</v>
-      </c>
-      <c r="G131" t="s">
-        <v>12</v>
-      </c>
-      <c r="H131" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8">
-      <c r="A132" t="s">
-        <v>373</v>
-      </c>
-      <c r="B132" t="s">
-        <v>85</v>
-      </c>
-      <c r="C132">
-        <v>1</v>
-      </c>
-      <c r="D132">
-        <v>376.0</v>
-      </c>
-      <c r="E132" t="s">
-        <v>54</v>
-      </c>
-      <c r="F132" t="s">
-        <v>31</v>
-      </c>
-      <c r="G132" t="s">
-        <v>12</v>
-      </c>
-      <c r="H132" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8">
-      <c r="A133" t="s">
-        <v>375</v>
-      </c>
-      <c r="B133" t="s">
-        <v>72</v>
-      </c>
-      <c r="C133">
-        <v>1</v>
-      </c>
-      <c r="D133">
-        <v>396.0</v>
-      </c>
-      <c r="E133" t="s">
-        <v>82</v>
-      </c>
-      <c r="F133" t="s">
-        <v>31</v>
-      </c>
-      <c r="G133" t="s">
-        <v>20</v>
-      </c>
-      <c r="H133" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8">
-      <c r="A134" t="s">
-        <v>377</v>
-      </c>
-      <c r="B134" t="s">
-        <v>186</v>
-      </c>
-      <c r="C134">
-        <v>1</v>
-      </c>
-      <c r="D134">
-        <v>475.0</v>
-      </c>
-      <c r="E134" t="s">
-        <v>363</v>
-      </c>
-      <c r="F134" t="s">
-        <v>31</v>
-      </c>
-      <c r="G134" t="s">
-        <v>144</v>
-      </c>
-      <c r="H134" t="s">
-        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -5084,13 +4854,6 @@
     <hyperlink ref="A125" r:id="rId_hyperlink_124"/>
     <hyperlink ref="A126" r:id="rId_hyperlink_125"/>
     <hyperlink ref="A127" r:id="rId_hyperlink_126"/>
-    <hyperlink ref="A128" r:id="rId_hyperlink_127"/>
-    <hyperlink ref="A129" r:id="rId_hyperlink_128"/>
-    <hyperlink ref="A130" r:id="rId_hyperlink_129"/>
-    <hyperlink ref="A131" r:id="rId_hyperlink_130"/>
-    <hyperlink ref="A132" r:id="rId_hyperlink_131"/>
-    <hyperlink ref="A133" r:id="rId_hyperlink_132"/>
-    <hyperlink ref="A134" r:id="rId_hyperlink_133"/>
   </hyperlinks>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>